<commit_message>
Add fire name and year to the studies table
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
+++ b/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDC35B0-9EEB-784B-9437-B24B4299C8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00337E84-FDA5-7E42-8B09-37769283A9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="4" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6479" uniqueCount="1509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6512" uniqueCount="1534">
   <si>
     <t>Study</t>
   </si>
@@ -4712,6 +4712,81 @@
   </si>
   <si>
     <t>The USGS gauges that they list in the paper dont have Q. This is the closest one I could find from their website. F Flathead River Near West Glacier MT - 12358500</t>
+  </si>
+  <si>
+    <t>Fire_name</t>
+  </si>
+  <si>
+    <t>Jesusita Fire</t>
+  </si>
+  <si>
+    <t>Hewlett Gulch_High Park fire</t>
+  </si>
+  <si>
+    <t>Hayman Fire (2002)</t>
+  </si>
+  <si>
+    <t>High Park Fire (2012)</t>
+  </si>
+  <si>
+    <t>Yosemite NP Fire</t>
+  </si>
+  <si>
+    <t>Caldor Fire(2021)_Mosquito Fire (2002)</t>
+  </si>
+  <si>
+    <t>Angora Fire (2007)</t>
+  </si>
+  <si>
+    <t>Anaktuvuk River wildfire (2007)</t>
+  </si>
+  <si>
+    <t>Thompson Ridge Wildfire (2013)</t>
+  </si>
+  <si>
+    <t>Boundary Fire (2004)</t>
+  </si>
+  <si>
+    <t>Lost Creek Wildfire (2003)</t>
+  </si>
+  <si>
+    <t>Camp Branch Fire (2016)_Tellico Fire (2016)</t>
+  </si>
+  <si>
+    <t>Clover-Mist Wildfire (1988)</t>
+  </si>
+  <si>
+    <t>Historic Fires</t>
+  </si>
+  <si>
+    <t>Rampage Fire (2003)_Others in Glacier NP</t>
+  </si>
+  <si>
+    <t>Fern Lake (2012)</t>
+  </si>
+  <si>
+    <t>Fourmile Canyon Fire (2010)</t>
+  </si>
+  <si>
+    <t>Rocky Fire (2015)_Wragg Fire (2015)</t>
+  </si>
+  <si>
+    <t>Hayman Fire (2002)_High Park Fire (2012)</t>
+  </si>
+  <si>
+    <t>No name given (2002)</t>
+  </si>
+  <si>
+    <t>Northwest Territories Fire (2013)</t>
+  </si>
+  <si>
+    <t>Red Bench Fire (1988)</t>
+  </si>
+  <si>
+    <t>No name given (2007)</t>
+  </si>
+  <si>
+    <t>Gaviota Fire (2004)</t>
   </si>
 </sst>
 </file>
@@ -5020,7 +5095,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -5180,6 +5255,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -27617,7 +27693,7 @@
   <dimension ref="A1:AA42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
@@ -30028,24 +30104,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E83DAFB-3D69-1A4C-8997-3EF8B4236F27}">
-  <dimension ref="A1:AC34"/>
+  <dimension ref="A1:AD34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X3" sqref="X3"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="21" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="37.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="22" width="10.83203125" customWidth="1"/>
+    <col min="23" max="23" width="9.6640625" customWidth="1"/>
+    <col min="24" max="24" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1379</v>
       </c>
@@ -30074,67 +30151,70 @@
         <v>691</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>1509</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="74" t="s">
+      <c r="W1" s="74" t="s">
         <v>1380</v>
       </c>
-      <c r="W1" s="105" t="s">
+      <c r="X1" s="105" t="s">
         <v>1421</v>
       </c>
-      <c r="X1" s="105" t="s">
+      <c r="Y1" s="105" t="s">
         <v>1420</v>
       </c>
-      <c r="Y1" s="105" t="s">
+      <c r="Z1" s="105" t="s">
         <v>1457</v>
       </c>
-      <c r="Z1" s="105" t="s">
+      <c r="AA1" s="105" t="s">
         <v>1492</v>
       </c>
-      <c r="AA1" s="105" t="s">
+      <c r="AB1" s="105" t="s">
         <v>1465</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>1480</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>1487</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1243</v>
       </c>
@@ -30163,28 +30243,29 @@
       <c r="L2" s="60"/>
       <c r="M2" s="60"/>
       <c r="N2" s="60"/>
-      <c r="P2" s="60"/>
+      <c r="O2" s="60"/>
       <c r="Q2" s="60"/>
       <c r="R2" s="60"/>
       <c r="S2" s="60"/>
       <c r="T2" s="60"/>
-      <c r="U2" s="60" t="s">
+      <c r="U2" s="60"/>
+      <c r="V2" s="60" t="s">
         <v>682</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>1406</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>1156</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>1156</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1243</v>
       </c>
@@ -30213,58 +30294,61 @@
         <v>693</v>
       </c>
       <c r="J3" t="s">
+        <v>1512</v>
+      </c>
+      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>694</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>19</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>695</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>39.177683000000002</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>-105.26552</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>5</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>690</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>22</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>696</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>1382</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>1439</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>1438</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>1156</v>
       </c>
-      <c r="Z3" s="115" t="s">
+      <c r="AA3" s="115" t="s">
         <v>1494</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>1156</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1243</v>
       </c>
@@ -30293,55 +30377,58 @@
         <v>785</v>
       </c>
       <c r="J4" t="s">
+        <v>1512</v>
+      </c>
+      <c r="K4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>694</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>19</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>721</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>39.177683000000002</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>-105.26552</v>
-      </c>
-      <c r="S4" t="s">
-        <v>22</v>
       </c>
       <c r="T4" t="s">
         <v>22</v>
       </c>
       <c r="U4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" t="s">
         <v>1108</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>1382</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>1440</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>1441</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>1156</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>1495</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>1156</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1243</v>
       </c>
@@ -30370,46 +30457,49 @@
         <v>785</v>
       </c>
       <c r="J5" t="s">
+        <v>1513</v>
+      </c>
+      <c r="K5" t="s">
         <v>24</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>721</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>39.177683000000002</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>-105.26552</v>
-      </c>
-      <c r="S5" t="s">
-        <v>22</v>
       </c>
       <c r="T5" t="s">
         <v>22</v>
       </c>
       <c r="U5" t="s">
+        <v>22</v>
+      </c>
+      <c r="V5" t="s">
         <v>1107</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>1384</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>1426</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>1456</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>1156</v>
       </c>
-      <c r="Z5" s="116" t="s">
+      <c r="AA5" s="116" t="s">
         <v>1493</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>1156</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1243</v>
       </c>
@@ -30438,52 +30528,55 @@
         <v>785</v>
       </c>
       <c r="J6" t="s">
+        <v>1514</v>
+      </c>
+      <c r="K6" t="s">
         <v>873</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>926</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>927</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>37.534036999999998</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>-119.389139</v>
-      </c>
-      <c r="S6" t="s">
-        <v>22</v>
       </c>
       <c r="T6" t="s">
         <v>22</v>
       </c>
       <c r="U6" t="s">
+        <v>22</v>
+      </c>
+      <c r="V6" t="s">
         <v>925</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>1401</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>1426</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>1427</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>1156</v>
       </c>
-      <c r="Z6" s="116" t="s">
+      <c r="AA6" s="116" t="s">
         <v>1496</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>1156</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>1484</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1243</v>
       </c>
@@ -30508,50 +30601,53 @@
       <c r="I7" t="s">
         <v>785</v>
       </c>
-      <c r="M7" t="s">
+      <c r="J7" t="s">
+        <v>1529</v>
+      </c>
+      <c r="N7" t="s">
         <v>930</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>949</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>44.578524999999999</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>-115.66604</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>4</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>22</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>950</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>1386</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>1426</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>1427</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>1156</v>
       </c>
-      <c r="Z7" s="116" t="s">
+      <c r="AA7" s="116" t="s">
         <v>1497</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>1156</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1243</v>
       </c>
@@ -30579,50 +30675,53 @@
       <c r="I8" t="s">
         <v>785</v>
       </c>
-      <c r="M8">
+      <c r="J8" t="s">
+        <v>1530</v>
+      </c>
+      <c r="N8">
         <v>3</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>836</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>61.4</v>
       </c>
-      <c r="P8">
-        <v>121.433333</v>
-      </c>
       <c r="Q8">
+        <v>-121.433333</v>
+      </c>
+      <c r="R8">
         <v>0.5</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>743</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>22</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>837</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>1382</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>1424</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>1453</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>1156</v>
       </c>
-      <c r="Z8" s="116" t="s">
+      <c r="AA8" s="116" t="s">
         <v>1500</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>1156</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1243</v>
       </c>
@@ -30651,58 +30750,61 @@
         <v>785</v>
       </c>
       <c r="J9" t="s">
+        <v>1531</v>
+      </c>
+      <c r="K9" t="s">
         <v>24</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>724</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>19</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>725</v>
       </c>
-      <c r="O9" s="99">
+      <c r="P9" s="99">
         <v>48.762999999999998</v>
       </c>
-      <c r="P9" s="99">
+      <c r="Q9" s="99">
         <v>-114.226</v>
       </c>
-      <c r="Q9" s="100">
+      <c r="R9" s="100">
         <v>5</v>
       </c>
-      <c r="R9" s="100" t="s">
+      <c r="S9" s="100" t="s">
         <v>726</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>22</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>1395</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>1401</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>1424</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>1419</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>1156</v>
       </c>
-      <c r="Z9" s="116" t="s">
+      <c r="AA9" s="116" t="s">
         <v>1498</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>1156</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1243</v>
       </c>
@@ -30731,58 +30833,61 @@
         <v>785</v>
       </c>
       <c r="J10" t="s">
+        <v>1515</v>
+      </c>
+      <c r="K10" t="s">
         <v>1168</v>
       </c>
-      <c r="L10" s="46" t="s">
+      <c r="M10" s="46" t="s">
         <v>1166</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>987</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>1167</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>38.916015999999999</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>-120.281718</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>2</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>1170</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>22</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>1169</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>1382</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>1424</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>1434</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>1156</v>
       </c>
-      <c r="Z10" s="116" t="s">
+      <c r="AA10" s="116" t="s">
         <v>1500</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>1156</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1243</v>
       </c>
@@ -30811,49 +30916,52 @@
         <v>785</v>
       </c>
       <c r="J11" t="s">
+        <v>1516</v>
+      </c>
+      <c r="K11" t="s">
         <v>882</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>883</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>884</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>38.896382000000003</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>-120.041629</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>2</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>22</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>887</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>1401</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>1424</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>1499</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>1458</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>1156</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1243</v>
       </c>
@@ -30881,50 +30989,53 @@
       <c r="I12" t="s">
         <v>785</v>
       </c>
-      <c r="M12" t="s">
+      <c r="J12" t="s">
+        <v>1517</v>
+      </c>
+      <c r="N12" t="s">
         <v>937</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>938</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>69.166667000000004</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>-150.75</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>2</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>22</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>939</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>1382</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>1432</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>1431</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>1459</v>
       </c>
-      <c r="Z12" s="116" t="s">
+      <c r="AA12" s="116" t="s">
         <v>1500</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>1482</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1243</v>
       </c>
@@ -30939,26 +31050,29 @@
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="V13" t="s">
+      <c r="J13" t="s">
+        <v>1510</v>
+      </c>
+      <c r="W13" t="s">
         <v>1450</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>1455</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>1454</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>1244</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>1156</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1243</v>
       </c>
@@ -30986,56 +31100,59 @@
       <c r="I14" t="s">
         <v>692</v>
       </c>
-      <c r="L14" t="s">
+      <c r="J14" s="106" t="s">
+        <v>1518</v>
+      </c>
+      <c r="M14" t="s">
         <v>1176</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>1177</v>
       </c>
-      <c r="N14" s="106" t="s">
+      <c r="O14" s="106" t="s">
         <v>1175</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>35.890813000000001</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>-106.540854</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>9</v>
-      </c>
-      <c r="S14" t="s">
-        <v>22</v>
       </c>
       <c r="T14" t="s">
         <v>22</v>
       </c>
       <c r="U14" t="s">
+        <v>22</v>
+      </c>
+      <c r="V14" t="s">
         <v>1178</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>1390</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>1422</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>1433</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>1464</v>
       </c>
-      <c r="Z14" s="116" t="s">
+      <c r="AA14" s="116" t="s">
         <v>1500</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>1481</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>1484</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1243</v>
       </c>
@@ -31063,59 +31180,62 @@
       <c r="I15" t="s">
         <v>692</v>
       </c>
-      <c r="J15" s="93" t="s">
+      <c r="J15" t="s">
+        <v>1156</v>
+      </c>
+      <c r="K15" s="93" t="s">
         <v>733</v>
       </c>
-      <c r="K15" s="93" t="s">
+      <c r="L15" s="93" t="s">
         <v>734</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="93" t="s">
+      <c r="O15" s="93" t="s">
         <v>731</v>
       </c>
-      <c r="O15" s="94">
+      <c r="P15" s="94">
         <v>49.667000000000002</v>
       </c>
-      <c r="P15" s="94">
+      <c r="Q15" s="94">
         <v>-93.733000000000004</v>
       </c>
-      <c r="Q15" s="95">
+      <c r="R15" s="95">
         <v>15</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>732</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>22</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>1394</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>1390</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>1422</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>1414</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>1244</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>1500</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>1156</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1243</v>
       </c>
@@ -31143,56 +31263,59 @@
       <c r="I16" t="s">
         <v>693</v>
       </c>
-      <c r="L16" t="s">
+      <c r="J16" t="s">
+        <v>1519</v>
+      </c>
+      <c r="M16" t="s">
         <v>19</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>784</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>783</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>65.150000000000006</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>-147.5</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>3</v>
-      </c>
-      <c r="S16" t="s">
-        <v>22</v>
       </c>
       <c r="T16" t="s">
         <v>22</v>
       </c>
       <c r="U16" t="s">
+        <v>22</v>
+      </c>
+      <c r="V16" t="s">
         <v>782</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>1405</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>1422</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>1415</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>1460</v>
       </c>
-      <c r="Z16" s="116" t="s">
+      <c r="AA16" s="116" t="s">
         <v>1501</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AC16" t="s">
         <v>1156</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AD16" t="s">
         <v>1484</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1243</v>
       </c>
@@ -31221,58 +31344,61 @@
         <v>785</v>
       </c>
       <c r="J17" t="s">
+        <v>1520</v>
+      </c>
+      <c r="K17" t="s">
         <v>24</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>741</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>19</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>742</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>49.616667</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>-114.666667</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>3</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>744</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>22</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>1393</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>1401</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>1422</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>1416</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>1461</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>1502</v>
       </c>
-      <c r="AB17" s="114" t="s">
+      <c r="AC17" s="114" t="s">
         <v>1156</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AD17" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1243</v>
       </c>
@@ -31298,58 +31424,61 @@
         <v>785</v>
       </c>
       <c r="J18" t="s">
+        <v>1521</v>
+      </c>
+      <c r="K18" t="s">
         <v>1004</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>1002</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>1378</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>35</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>-83</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>2</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>989</v>
-      </c>
-      <c r="S18" t="s">
-        <v>22</v>
       </c>
       <c r="T18" t="s">
         <v>22</v>
       </c>
       <c r="U18" t="s">
+        <v>22</v>
+      </c>
+      <c r="V18" t="s">
         <v>1005</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>1382</v>
       </c>
-      <c r="W18" t="s">
+      <c r="X18" t="s">
         <v>1422</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>1503</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>1462</v>
       </c>
-      <c r="Z18" s="116" t="s">
+      <c r="AA18" s="116" t="s">
         <v>1504</v>
       </c>
-      <c r="AB18" s="113" t="s">
+      <c r="AC18" s="113" t="s">
         <v>1156</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AD18" t="s">
         <v>1484</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1243</v>
       </c>
@@ -31374,53 +31503,56 @@
       <c r="I19" t="s">
         <v>785</v>
       </c>
-      <c r="M19" t="s">
+      <c r="J19" t="s">
+        <v>1512</v>
+      </c>
+      <c r="N19" t="s">
         <v>985</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>695</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>39.177683000000002</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>-105.26552</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>2</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>984</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>22</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>983</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>1401</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>1422</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>1417</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>1463</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AA19" t="s">
         <v>1500</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AC19" t="s">
         <v>1483</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AD19" t="s">
         <v>1484</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1243</v>
       </c>
@@ -31435,32 +31567,35 @@
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
-      <c r="V20" t="s">
+      <c r="J20" t="s">
+        <v>1533</v>
+      </c>
+      <c r="W20" t="s">
         <v>1401</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>1422</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Y20" t="s">
         <v>1445</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>1466</v>
       </c>
-      <c r="Z20" s="116" t="s">
+      <c r="AA20" s="116" t="s">
         <v>1505</v>
       </c>
-      <c r="AA20" s="62" t="s">
+      <c r="AB20" s="62" t="s">
         <v>1467</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AC20" t="s">
         <v>1156</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AD20" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1243</v>
       </c>
@@ -31489,61 +31624,64 @@
         <v>785</v>
       </c>
       <c r="J21" t="s">
+        <v>1522</v>
+      </c>
+      <c r="K21" t="s">
         <v>24</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>932</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>930</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>931</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>44.512999999999998</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>-109.98</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>4</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>933</v>
-      </c>
-      <c r="S21" t="s">
-        <v>22</v>
       </c>
       <c r="T21" t="s">
         <v>22</v>
       </c>
       <c r="U21" t="s">
+        <v>22</v>
+      </c>
+      <c r="V21" t="s">
         <v>934</v>
       </c>
-      <c r="V21" t="s">
+      <c r="W21" t="s">
         <v>1382</v>
       </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
         <v>1422</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>1468</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>1469</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="AA21" t="s">
         <v>1500</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AC21" t="s">
         <v>1156</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="AD21" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1243</v>
       </c>
@@ -31558,32 +31696,35 @@
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
-      <c r="V22" t="s">
+      <c r="J22" t="s">
+        <v>1523</v>
+      </c>
+      <c r="W22" t="s">
         <v>1381</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>1422</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>1470</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>1471</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
         <v>1506</v>
       </c>
-      <c r="AA22" s="114" t="s">
+      <c r="AB22" s="114" t="s">
         <v>1472</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AC22" t="s">
         <v>1156</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AD22" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1243</v>
       </c>
@@ -31612,50 +31753,53 @@
         <v>785</v>
       </c>
       <c r="J23" t="s">
+        <v>1532</v>
+      </c>
+      <c r="K23" t="s">
         <v>1184</v>
       </c>
-      <c r="K23" s="97"/>
-      <c r="M23">
+      <c r="L23" s="97"/>
+      <c r="N23">
         <v>4</v>
       </c>
-      <c r="N23" s="98" t="s">
+      <c r="O23" s="98" t="s">
         <v>1186</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>44.910800000000002</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>-116.1031</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>22</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>1185</v>
       </c>
-      <c r="V23" t="s">
+      <c r="W23" t="s">
         <v>1401</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>1422</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>1418</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>1473</v>
       </c>
-      <c r="Z23" t="s">
+      <c r="AA23" t="s">
         <v>1507</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AC23" t="s">
         <v>1156</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="AD23" t="s">
         <v>1485</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1243</v>
       </c>
@@ -31683,63 +31827,66 @@
       <c r="I24" s="102" t="s">
         <v>785</v>
       </c>
-      <c r="J24" s="93" t="s">
+      <c r="J24" s="117" t="s">
+        <v>1524</v>
+      </c>
+      <c r="K24" s="93" t="s">
         <v>751</v>
       </c>
-      <c r="K24" s="93" t="s">
+      <c r="L24" s="93" t="s">
         <v>752</v>
       </c>
-      <c r="L24" s="93" t="s">
+      <c r="M24" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="M24" s="96"/>
-      <c r="N24" s="93" t="s">
+      <c r="N24" s="96"/>
+      <c r="O24" s="93" t="s">
         <v>753</v>
       </c>
-      <c r="O24" s="94">
+      <c r="P24" s="94">
         <v>48.789253000000002</v>
       </c>
-      <c r="P24" s="94">
+      <c r="Q24" s="94">
         <v>-113.79626500000001</v>
       </c>
-      <c r="Q24" s="95">
+      <c r="R24" s="95">
         <v>4</v>
       </c>
-      <c r="R24" s="95" t="s">
+      <c r="S24" s="95" t="s">
         <v>754</v>
-      </c>
-      <c r="S24" s="96" t="s">
-        <v>22</v>
       </c>
       <c r="T24" s="96" t="s">
         <v>22</v>
       </c>
       <c r="U24" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="V24" s="96" t="s">
         <v>1392</v>
       </c>
-      <c r="V24" s="96" t="s">
+      <c r="W24" s="96" t="s">
         <v>1403</v>
       </c>
-      <c r="W24" s="96" t="s">
+      <c r="X24" s="96" t="s">
         <v>1422</v>
       </c>
-      <c r="X24" s="96" t="s">
+      <c r="Y24" s="96" t="s">
         <v>1474</v>
       </c>
-      <c r="Y24" s="96" t="s">
+      <c r="Z24" s="96" t="s">
         <v>1475</v>
       </c>
-      <c r="Z24" s="116" t="s">
+      <c r="AA24" s="116" t="s">
         <v>1508</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AC24" t="s">
         <v>1156</v>
       </c>
-      <c r="AC24" t="s">
+      <c r="AD24" t="s">
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1243</v>
       </c>
@@ -31767,65 +31914,68 @@
       <c r="I25" s="96" t="s">
         <v>693</v>
       </c>
-      <c r="J25" s="93" t="s">
+      <c r="J25" s="96" t="s">
+        <v>1525</v>
+      </c>
+      <c r="K25" s="93" t="s">
         <v>827</v>
       </c>
-      <c r="K25" s="93" t="s">
+      <c r="L25" s="93" t="s">
         <v>828</v>
       </c>
-      <c r="L25" s="93" t="s">
+      <c r="M25" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="M25" s="103" t="s">
+      <c r="N25" s="103" t="s">
         <v>833</v>
       </c>
-      <c r="N25" s="93" t="s">
+      <c r="O25" s="93" t="s">
         <v>829</v>
       </c>
-      <c r="O25" s="94">
+      <c r="P25" s="94">
         <v>40.353888888</v>
       </c>
-      <c r="P25" s="94">
+      <c r="Q25" s="94">
         <v>-105.583611111</v>
       </c>
-      <c r="Q25" s="95">
+      <c r="R25" s="95">
         <v>2</v>
       </c>
-      <c r="R25" s="95" t="s">
+      <c r="S25" s="95" t="s">
         <v>830</v>
-      </c>
-      <c r="S25" s="96" t="s">
-        <v>22</v>
       </c>
       <c r="T25" s="96" t="s">
         <v>22</v>
       </c>
       <c r="U25" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="V25" s="96" t="s">
         <v>831</v>
       </c>
-      <c r="V25" t="s">
+      <c r="W25" t="s">
         <v>1405</v>
       </c>
-      <c r="W25" t="s">
+      <c r="X25" t="s">
         <v>1422</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" t="s">
         <v>1423</v>
       </c>
-      <c r="Y25" s="96" t="s">
+      <c r="Z25" s="96" t="s">
         <v>1476</v>
       </c>
-      <c r="Z25" s="96" t="s">
+      <c r="AA25" s="96" t="s">
         <v>1500</v>
       </c>
-      <c r="AB25" t="s">
+      <c r="AC25" t="s">
         <v>1156</v>
       </c>
-      <c r="AC25" t="s">
+      <c r="AD25" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1243</v>
       </c>
@@ -31853,54 +32003,57 @@
       <c r="I26" t="s">
         <v>785</v>
       </c>
-      <c r="L26" t="s">
+      <c r="J26" s="96" t="s">
+        <v>1526</v>
+      </c>
+      <c r="M26" t="s">
         <v>19</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>708</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>40.033332999999999</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>-105.416667</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>3</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>709</v>
-      </c>
-      <c r="S26" t="s">
-        <v>22</v>
       </c>
       <c r="T26" t="s">
         <v>22</v>
       </c>
       <c r="U26" t="s">
+        <v>22</v>
+      </c>
+      <c r="V26" t="s">
         <v>710</v>
       </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>1382</v>
       </c>
-      <c r="W26" t="s">
+      <c r="X26" t="s">
         <v>1422</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Y26" t="s">
         <v>1435</v>
       </c>
-      <c r="Y26" s="96" t="s">
+      <c r="Z26" s="96" t="s">
         <v>1477</v>
       </c>
-      <c r="Z26" s="96"/>
-      <c r="AB26" t="s">
+      <c r="AA26" s="96"/>
+      <c r="AC26" t="s">
         <v>1156</v>
       </c>
-      <c r="AC26" t="s">
+      <c r="AD26" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1243</v>
       </c>
@@ -31922,53 +32075,56 @@
       <c r="G27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M27" t="s">
+      <c r="J27" s="96" t="s">
+        <v>1526</v>
+      </c>
+      <c r="N27" t="s">
         <v>849</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>1377</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>40.050263700000002</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>-105.3666599</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>5</v>
-      </c>
-      <c r="S27" t="s">
-        <v>22</v>
       </c>
       <c r="T27" t="s">
         <v>22</v>
       </c>
       <c r="U27" t="s">
+        <v>22</v>
+      </c>
+      <c r="V27" t="s">
         <v>850</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>1401</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>1422</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>1425</v>
       </c>
-      <c r="Y27" s="96" t="s">
+      <c r="Z27" s="96" t="s">
         <v>1477</v>
       </c>
-      <c r="Z27" s="96" t="s">
+      <c r="AA27" s="96" t="s">
         <v>1500</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AC27" t="s">
         <v>1156</v>
       </c>
-      <c r="AC27" t="s">
+      <c r="AD27" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1243</v>
       </c>
@@ -31996,57 +32152,60 @@
       <c r="I28" t="s">
         <v>785</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="96" t="s">
+        <v>1527</v>
+      </c>
+      <c r="K28" t="s">
         <v>873</v>
       </c>
-      <c r="M28" s="104" t="s">
+      <c r="N28" s="104" t="s">
         <v>874</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>875</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>38.512031</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>-122.097228</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>3</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>876</v>
-      </c>
-      <c r="S28" t="s">
-        <v>22</v>
       </c>
       <c r="T28" t="s">
         <v>22</v>
       </c>
       <c r="U28" t="s">
+        <v>22</v>
+      </c>
+      <c r="V28" t="s">
         <v>872</v>
       </c>
-      <c r="V28" t="s">
+      <c r="W28" t="s">
         <v>1401</v>
       </c>
-      <c r="W28" t="s">
+      <c r="X28" t="s">
         <v>1422</v>
       </c>
-      <c r="X28" t="s">
+      <c r="Y28" t="s">
         <v>1428</v>
       </c>
-      <c r="Y28" s="96" t="s">
+      <c r="Z28" s="96" t="s">
         <v>1478</v>
       </c>
-      <c r="Z28" s="96"/>
-      <c r="AB28" t="s">
+      <c r="AA28" s="96"/>
+      <c r="AC28" t="s">
         <v>1156</v>
       </c>
-      <c r="AC28" t="s">
+      <c r="AD28" t="s">
         <v>1488</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1243</v>
       </c>
@@ -32059,24 +32218,27 @@
       <c r="D29" t="s">
         <v>1451</v>
       </c>
-      <c r="W29" t="s">
+      <c r="J29" s="96" t="s">
+        <v>1526</v>
+      </c>
+      <c r="X29" t="s">
         <v>1422</v>
       </c>
-      <c r="X29" t="s">
+      <c r="Y29" t="s">
         <v>1452</v>
       </c>
-      <c r="Y29" s="96" t="s">
+      <c r="Z29" s="96" t="s">
         <v>1479</v>
       </c>
-      <c r="Z29" s="96"/>
-      <c r="AB29" t="s">
+      <c r="AA29" s="96"/>
+      <c r="AC29" t="s">
         <v>1156</v>
       </c>
-      <c r="AC29" t="s">
+      <c r="AD29" t="s">
         <v>1489</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1243</v>
       </c>
@@ -32091,30 +32253,33 @@
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
-      <c r="L30" s="46"/>
-      <c r="V30" t="s">
+      <c r="J30" t="s">
+        <v>1511</v>
+      </c>
+      <c r="M30" s="46"/>
+      <c r="W30" t="s">
         <v>1390</v>
       </c>
-      <c r="W30" t="s">
+      <c r="X30" t="s">
         <v>1430</v>
       </c>
-      <c r="X30" s="112" t="s">
+      <c r="Y30" s="112" t="s">
         <v>1448</v>
       </c>
-      <c r="Y30" s="96" t="s">
+      <c r="Z30" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z30" s="96" t="s">
+      <c r="AA30" s="96" t="s">
         <v>1493</v>
       </c>
-      <c r="AB30" t="s">
+      <c r="AC30" t="s">
         <v>1156</v>
       </c>
-      <c r="AC30" t="s">
+      <c r="AD30" t="s">
         <v>1490</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>1243</v>
       </c>
@@ -32142,62 +32307,65 @@
       <c r="I31" t="s">
         <v>785</v>
       </c>
-      <c r="J31" s="108" t="s">
+      <c r="J31" t="s">
+        <v>1513</v>
+      </c>
+      <c r="K31" s="108" t="s">
         <v>770</v>
       </c>
-      <c r="K31" s="108" t="s">
+      <c r="L31" s="108" t="s">
         <v>771</v>
       </c>
-      <c r="L31" s="108" t="s">
+      <c r="M31" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>1</v>
       </c>
-      <c r="N31" s="108" t="s">
+      <c r="O31" s="108" t="s">
         <v>767</v>
       </c>
-      <c r="O31" s="109">
+      <c r="P31" s="109">
         <v>40.7159999</v>
       </c>
-      <c r="P31" s="109">
+      <c r="Q31" s="109">
         <v>-105.23308400000001</v>
       </c>
-      <c r="Q31" s="110">
+      <c r="R31" s="110">
         <v>0.5</v>
       </c>
-      <c r="R31" s="110" t="s">
+      <c r="S31" s="110" t="s">
         <v>768</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>22</v>
       </c>
-      <c r="U31" t="s">
+      <c r="V31" t="s">
         <v>769</v>
       </c>
-      <c r="V31" t="s">
+      <c r="W31" t="s">
         <v>1382</v>
       </c>
-      <c r="W31" t="s">
+      <c r="X31" t="s">
         <v>1430</v>
       </c>
-      <c r="X31" t="s">
+      <c r="Y31" t="s">
         <v>1442</v>
       </c>
-      <c r="Y31" s="96" t="s">
+      <c r="Z31" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z31" s="96" t="s">
+      <c r="AA31" s="96" t="s">
         <v>1493</v>
       </c>
-      <c r="AB31" t="s">
+      <c r="AC31" t="s">
         <v>1156</v>
       </c>
-      <c r="AC31" t="s">
+      <c r="AD31" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>1243</v>
       </c>
@@ -32222,63 +32390,66 @@
       <c r="I32" t="s">
         <v>785</v>
       </c>
-      <c r="J32" s="96" t="s">
+      <c r="J32" t="s">
+        <v>1511</v>
+      </c>
+      <c r="K32" s="96" t="s">
         <v>770</v>
       </c>
-      <c r="K32" s="96" t="s">
+      <c r="L32" s="96" t="s">
         <v>771</v>
       </c>
-      <c r="L32" s="96" t="s">
+      <c r="M32" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="M32" s="96"/>
-      <c r="N32" s="96" t="s">
+      <c r="N32" s="96"/>
+      <c r="O32" s="96" t="s">
         <v>767</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>40.702464999999997</v>
       </c>
-      <c r="P32">
+      <c r="Q32">
         <v>-105.241646</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>1</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>790</v>
-      </c>
-      <c r="S32" t="s">
-        <v>22</v>
       </c>
       <c r="T32" t="s">
         <v>22</v>
       </c>
       <c r="U32" t="s">
+        <v>22</v>
+      </c>
+      <c r="V32" t="s">
         <v>791</v>
       </c>
-      <c r="V32" t="s">
+      <c r="W32" t="s">
         <v>1401</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>1430</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>1429</v>
       </c>
-      <c r="Y32" s="96" t="s">
+      <c r="Z32" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z32" s="96" t="s">
+      <c r="AA32" s="96" t="s">
         <v>1493</v>
       </c>
-      <c r="AB32" t="s">
+      <c r="AC32" t="s">
         <v>1156</v>
       </c>
-      <c r="AC32" t="s">
+      <c r="AD32" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1243</v>
       </c>
@@ -32293,31 +32464,34 @@
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
-      <c r="K33" s="97"/>
-      <c r="N33" s="98"/>
-      <c r="V33" t="s">
+      <c r="J33" t="s">
+        <v>1512</v>
+      </c>
+      <c r="L33" s="97"/>
+      <c r="O33" s="98"/>
+      <c r="W33" t="s">
         <v>1385</v>
       </c>
-      <c r="W33" t="s">
+      <c r="X33" t="s">
         <v>1436</v>
       </c>
-      <c r="X33" t="s">
+      <c r="Y33" t="s">
         <v>1446</v>
       </c>
-      <c r="Y33" s="96" t="s">
+      <c r="Z33" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z33" s="96" t="s">
+      <c r="AA33" s="96" t="s">
         <v>1494</v>
       </c>
-      <c r="AB33" t="s">
+      <c r="AC33" t="s">
         <v>1156</v>
       </c>
-      <c r="AC33" t="s">
+      <c r="AD33" t="s">
         <v>1491</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1243</v>
       </c>
@@ -32346,57 +32520,60 @@
         <v>785</v>
       </c>
       <c r="J34" t="s">
+        <v>1528</v>
+      </c>
+      <c r="K34" t="s">
         <v>24</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>1094</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>1092</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>1093</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>1096</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>40.262369999999997</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <v>-105.59080400000001</v>
       </c>
-      <c r="Q34" s="100">
+      <c r="R34" s="100">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="U34" t="s">
+      <c r="V34" t="s">
         <v>1095</v>
       </c>
-      <c r="V34" t="s">
+      <c r="W34" t="s">
         <v>1382</v>
       </c>
-      <c r="W34" t="s">
+      <c r="X34" t="s">
         <v>1436</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Y34" t="s">
         <v>1437</v>
       </c>
-      <c r="Y34" s="96" t="s">
+      <c r="Z34" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z34" s="96" t="s">
+      <c r="AA34" s="96" t="s">
         <v>1494</v>
       </c>
-      <c r="AB34" t="s">
+      <c r="AC34" t="s">
         <v>1156</v>
       </c>
-      <c r="AC34" t="s">
+      <c r="AD34" t="s">
         <v>1491</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X34">
-    <sortCondition ref="W2:W34"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y34">
+    <sortCondition ref="X2:X34"/>
   </sortState>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G7 G19:G25" xr:uid="{8B21EFF3-D61C-024F-A87C-4FC0F83918E4}">

</xml_diff>

<commit_message>
Added Gluns and Toews from Hampton cross reference
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
+++ b/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDDFB94-116C-914B-92E9-B631C3D77709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C522339-8F7F-D546-BDA0-5C0807CC2E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="5" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="4" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
   </bookViews>
   <sheets>
     <sheet name="Study_info" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6638" uniqueCount="1597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="1606">
   <si>
     <t>Study</t>
   </si>
@@ -4977,6 +4977,33 @@
   </si>
   <si>
     <t>Added, but doesn’t have Q data</t>
+  </si>
+  <si>
+    <t>Gluns &amp; Toews, 1989</t>
+  </si>
+  <si>
+    <t>Effect of a major wildfire on water quality in southeastern British Columbia</t>
+  </si>
+  <si>
+    <t>Temperate coniferous forest</t>
+  </si>
+  <si>
+    <t>Western larch, Douglas fir, Engelman spruce, subalpine fir</t>
+  </si>
+  <si>
+    <t>Kimberley, BC, Canada</t>
+  </si>
+  <si>
+    <t>0 to 3</t>
+  </si>
+  <si>
+    <t>Figure 2 has a time series of Q for Mather Creek. L/s/km^2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 3 has nitrate-N for East fork (burned) middle fork (burned) and West Fork (unburned). Hampton has already extracted this data and Ill be using that </t>
+  </si>
+  <si>
+    <t>Matt fire, 1985</t>
   </si>
 </sst>
 </file>
@@ -5291,7 +5318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -5451,17 +5478,14 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -30310,11 +30334,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E83DAFB-3D69-1A4C-8997-3EF8B4236F27}">
-  <dimension ref="A1:AD35"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC35" sqref="AC35"/>
+      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32778,7 +32802,10 @@
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B35" s="125" t="s">
+      <c r="A35" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B35" s="93" t="s">
         <v>1588</v>
       </c>
       <c r="C35">
@@ -32805,10 +32832,10 @@
       <c r="O35" t="s">
         <v>1592</v>
       </c>
-      <c r="P35" s="126">
+      <c r="P35" s="122">
         <v>48.102674999999998</v>
       </c>
-      <c r="Q35" s="126">
+      <c r="Q35" s="122">
         <v>-120.35232000000001</v>
       </c>
       <c r="R35">
@@ -32831,6 +32858,53 @@
       </c>
       <c r="Y35" t="s">
         <v>1595</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C36">
+        <v>1989</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1598</v>
+      </c>
+      <c r="J36" t="s">
+        <v>1605</v>
+      </c>
+      <c r="K36" t="s">
+        <v>1599</v>
+      </c>
+      <c r="L36" t="s">
+        <v>1600</v>
+      </c>
+      <c r="N36" t="s">
+        <v>1602</v>
+      </c>
+      <c r="O36" t="s">
+        <v>1601</v>
+      </c>
+      <c r="P36" s="124">
+        <v>49.704340000000002</v>
+      </c>
+      <c r="Q36" s="124">
+        <v>-116.118877</v>
+      </c>
+      <c r="R36">
+        <v>3</v>
+      </c>
+      <c r="U36" t="s">
+        <v>22</v>
+      </c>
+      <c r="V36" t="s">
+        <v>1604</v>
+      </c>
+      <c r="X36" t="s">
+        <v>1422</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>1603</v>
       </c>
     </row>
   </sheetData>
@@ -32857,7 +32931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C183780A-8505-B94B-8F3A-3F461C5D9C3A}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -32901,7 +32975,7 @@
       <c r="B3" s="118" t="s">
         <v>1548</v>
       </c>
-      <c r="D3" s="119" t="s">
+      <c r="D3" s="60" t="s">
         <v>681</v>
       </c>
     </row>
@@ -32909,13 +32983,13 @@
       <c r="A4" s="69" t="s">
         <v>681</v>
       </c>
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="119" t="s">
         <v>1562</v>
       </c>
       <c r="C4" t="s">
         <v>1575</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" t="s">
         <v>1413</v>
       </c>
     </row>
@@ -32923,13 +32997,13 @@
       <c r="A5" t="s">
         <v>681</v>
       </c>
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="119" t="s">
         <v>1566</v>
       </c>
       <c r="C5" t="s">
         <v>1576</v>
       </c>
-      <c r="D5" s="120" t="s">
+      <c r="D5" t="s">
         <v>1443</v>
       </c>
     </row>
@@ -32940,7 +33014,7 @@
       <c r="B6" s="118" t="s">
         <v>1543</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" t="s">
         <v>928</v>
       </c>
     </row>
@@ -32948,13 +33022,13 @@
       <c r="A7" s="29" t="s">
         <v>1413</v>
       </c>
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="120" t="s">
         <v>1544</v>
       </c>
       <c r="C7" t="s">
         <v>1577</v>
       </c>
-      <c r="D7" s="120" t="s">
+      <c r="D7" t="s">
         <v>727</v>
       </c>
     </row>
@@ -32962,13 +33036,13 @@
       <c r="A8" t="s">
         <v>835</v>
       </c>
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="119" t="s">
         <v>1551</v>
       </c>
       <c r="C8" t="s">
         <v>1578</v>
       </c>
-      <c r="D8" s="120" t="s">
+      <c r="D8" t="s">
         <v>1231</v>
       </c>
     </row>
@@ -32976,13 +33050,13 @@
       <c r="A9" t="s">
         <v>1001</v>
       </c>
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="119" t="s">
         <v>1551</v>
       </c>
       <c r="C9" t="s">
         <v>1579</v>
       </c>
-      <c r="D9" s="120" t="s">
+      <c r="D9" t="s">
         <v>1233</v>
       </c>
     </row>
@@ -32990,13 +33064,13 @@
       <c r="A10" t="s">
         <v>982</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="119" t="s">
         <v>1563</v>
       </c>
       <c r="C10" t="s">
         <v>1580</v>
       </c>
-      <c r="D10" s="121" t="s">
+      <c r="D10" s="96" t="s">
         <v>750</v>
       </c>
     </row>
@@ -33004,13 +33078,13 @@
       <c r="A11" s="29" t="s">
         <v>1443</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="119" t="s">
         <v>1554</v>
       </c>
       <c r="C11" t="s">
         <v>1581</v>
       </c>
-      <c r="D11" s="121" t="s">
+      <c r="D11" s="96" t="s">
         <v>826</v>
       </c>
     </row>
@@ -33018,13 +33092,13 @@
       <c r="A12" s="29" t="s">
         <v>928</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="119" t="s">
         <v>1546</v>
       </c>
       <c r="C12" t="s">
         <v>1582</v>
       </c>
-      <c r="D12" s="120" t="s">
+      <c r="D12" t="s">
         <v>711</v>
       </c>
     </row>
@@ -33035,7 +33109,7 @@
       <c r="B13" s="118" t="s">
         <v>1558</v>
       </c>
-      <c r="D13" s="120" t="s">
+      <c r="D13" t="s">
         <v>881</v>
       </c>
     </row>
@@ -33043,13 +33117,13 @@
       <c r="A14" t="s">
         <v>909</v>
       </c>
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="121" t="s">
         <v>1564</v>
       </c>
       <c r="C14" t="s">
         <v>1586</v>
       </c>
-      <c r="D14" s="120" t="s">
+      <c r="D14" t="s">
         <v>762</v>
       </c>
     </row>
@@ -33060,7 +33134,7 @@
       <c r="B15" s="118" t="s">
         <v>1559</v>
       </c>
-      <c r="D15" s="120" t="s">
+      <c r="D15" t="s">
         <v>789</v>
       </c>
     </row>
@@ -33087,7 +33161,7 @@
       <c r="A18" s="29" t="s">
         <v>1231</v>
       </c>
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="119" t="s">
         <v>1570</v>
       </c>
       <c r="C18" t="s">
@@ -33101,7 +33175,7 @@
       <c r="A19" t="s">
         <v>720</v>
       </c>
-      <c r="B19" s="122" t="s">
+      <c r="B19" s="119" t="s">
         <v>1547</v>
       </c>
       <c r="C19" t="s">
@@ -33112,7 +33186,7 @@
       <c r="A20" s="29" t="s">
         <v>1233</v>
       </c>
-      <c r="B20" s="122" t="s">
+      <c r="B20" s="119" t="s">
         <v>1565</v>
       </c>
       <c r="C20" t="s">
@@ -33147,7 +33221,7 @@
       <c r="A24" t="s">
         <v>848</v>
       </c>
-      <c r="B24" s="124" t="s">
+      <c r="B24" s="121" t="s">
         <v>1567</v>
       </c>
       <c r="C24" t="s">
@@ -33166,7 +33240,7 @@
       <c r="A26" t="s">
         <v>1091</v>
       </c>
-      <c r="B26" s="122" t="s">
+      <c r="B26" s="119" t="s">
         <v>1555</v>
       </c>
       <c r="C26" t="s">
@@ -33196,7 +33270,7 @@
       <c r="A29" t="s">
         <v>924</v>
       </c>
-      <c r="B29" s="122" t="s">
+      <c r="B29" s="119" t="s">
         <v>1552</v>
       </c>
       <c r="C29" t="s">
@@ -33207,7 +33281,7 @@
       <c r="A30" t="s">
         <v>948</v>
       </c>
-      <c r="B30" s="122" t="s">
+      <c r="B30" s="119" t="s">
         <v>1556</v>
       </c>
       <c r="C30" t="s">
@@ -33218,7 +33292,7 @@
       <c r="A31" t="s">
         <v>871</v>
       </c>
-      <c r="B31" s="127" t="s">
+      <c r="B31" s="123" t="s">
         <v>1569</v>
       </c>
       <c r="C31" t="s">
@@ -33229,7 +33303,7 @@
       <c r="A32" t="s">
         <v>765</v>
       </c>
-      <c r="B32" s="122" t="s">
+      <c r="B32" s="119" t="s">
         <v>1557</v>
       </c>
       <c r="C32" t="s">
@@ -33240,7 +33314,7 @@
       <c r="A33" t="s">
         <v>1232</v>
       </c>
-      <c r="B33" s="122" t="s">
+      <c r="B33" s="119" t="s">
         <v>1553</v>
       </c>
       <c r="C33" t="s">
@@ -33251,7 +33325,7 @@
       <c r="A34" s="29" t="s">
         <v>789</v>
       </c>
-      <c r="B34" s="122" t="s">
+      <c r="B34" s="119" t="s">
         <v>1550</v>
       </c>
       <c r="C34" t="s">
@@ -33259,7 +33333,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B35" s="122" t="s">
+      <c r="B35" s="119" t="s">
         <v>1560</v>
       </c>
       <c r="C35" t="s">
@@ -33267,7 +33341,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B36" s="122" t="s">
+      <c r="B36" s="119" t="s">
         <v>1568</v>
       </c>
       <c r="C36" t="s">

</xml_diff>

<commit_message>
starting script to calculate percent difference with time
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
+++ b/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDA4D67-DD13-9F4B-9010-2DAF2910B7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E2221C-FBEF-F948-BDF3-567204A82F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="4" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6680" uniqueCount="1622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6680" uniqueCount="1621">
   <si>
     <t>Study</t>
   </si>
@@ -5037,9 +5037,6 @@
   </si>
   <si>
     <t>Y_mean_of_burn_reference</t>
-  </si>
-  <si>
-    <t>N_Cache_la_Poudre</t>
   </si>
   <si>
     <t>N_gave_a_range</t>
@@ -30383,9 +30380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E83DAFB-3D69-1A4C-8997-3EF8B4236F27}">
   <dimension ref="A1:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD37" sqref="AD37"/>
+      <selection pane="topRight" activeCell="AD35" sqref="AD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31772,7 +31769,7 @@
         <v>1489</v>
       </c>
       <c r="AD19" t="s">
-        <v>1617</v>
+        <v>1243</v>
       </c>
       <c r="AE19" t="s">
         <v>1243</v>
@@ -31812,7 +31809,7 @@
         <v>1243</v>
       </c>
       <c r="AD20" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="AE20" t="s">
         <v>1243</v>
@@ -32451,7 +32448,7 @@
         <v>1244</v>
       </c>
       <c r="AD28" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="AE28" t="s">
         <v>1243</v>
@@ -32614,7 +32611,7 @@
         <v>1483</v>
       </c>
       <c r="AD30" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="AE30" t="s">
         <v>1243</v>
@@ -32923,7 +32920,7 @@
         <v>1243</v>
       </c>
       <c r="AD34" t="s">
-        <v>1617</v>
+        <v>1243</v>
       </c>
       <c r="AE34" t="s">
         <v>1243</v>
@@ -32959,7 +32956,7 @@
         <v>1488</v>
       </c>
       <c r="AD35" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="AE35" t="s">
         <v>1243</v>

</xml_diff>

<commit_message>
updated script/added Crandall to list
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
+++ b/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72574A51-8A47-B14B-AE33-1BFB2956E610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26464C0-C9A9-814C-8FA2-3ACADE87BB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="4" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
+    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="4" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
   </bookViews>
   <sheets>
     <sheet name="Study_info" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6729" uniqueCount="1625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6741" uniqueCount="1630">
   <si>
     <t>Study</t>
   </si>
@@ -5062,6 +5062,21 @@
   <si>
     <t>N_pre_post</t>
   </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0257733</t>
+  </si>
+  <si>
+    <t>Utah Lake</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>Can only find TOC data to extract or take from the supplemental</t>
+  </si>
+  <si>
+    <t>Pole Creek Fire Complex</t>
+  </si>
 </sst>
 </file>
 
@@ -5070,7 +5085,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5292,6 +5307,11 @@
       <color rgb="FF1B1B1B"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="13">
@@ -5549,7 +5569,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5868,8 +5888,8 @@
   <dimension ref="A1:AQ321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30398,19 +30418,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E83DAFB-3D69-1A4C-8997-3EF8B4236F27}">
-  <dimension ref="A1:AG36"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X8" sqref="X8"/>
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="5" max="9" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="10" max="22" width="10.83203125" customWidth="1"/>
+    <col min="5" max="8" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="9" max="22" width="10.83203125" customWidth="1"/>
     <col min="23" max="23" width="9.6640625" customWidth="1"/>
     <col min="24" max="24" width="37.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="20.5" customWidth="1"/>
@@ -30520,7 +30540,7 @@
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="125" t="s">
         <v>935</v>
       </c>
       <c r="B2">
@@ -30600,7 +30620,7 @@
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="125" t="s">
         <v>1174</v>
       </c>
       <c r="B3">
@@ -30689,7 +30709,7 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="125" t="s">
         <v>681</v>
       </c>
       <c r="B4" s="60">
@@ -30746,7 +30766,7 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="125" t="s">
         <v>681</v>
       </c>
       <c r="B5">
@@ -30838,7 +30858,7 @@
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="125" t="s">
         <v>1404</v>
       </c>
       <c r="B6">
@@ -30927,7 +30947,7 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="125" t="s">
         <v>1413</v>
       </c>
       <c r="B7">
@@ -31016,7 +31036,7 @@
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="125" t="s">
         <v>835</v>
       </c>
       <c r="B8">
@@ -31099,7 +31119,7 @@
       </c>
     </row>
     <row r="9" spans="1:33" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="125" t="s">
         <v>1001</v>
       </c>
       <c r="B9">
@@ -31188,7 +31208,7 @@
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="125" t="s">
         <v>982</v>
       </c>
       <c r="B10">
@@ -31271,7 +31291,7 @@
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="125" t="s">
         <v>1443</v>
       </c>
       <c r="B11">
@@ -31320,56 +31340,40 @@
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>928</v>
+      <c r="A12" s="125" t="s">
+        <v>1115</v>
       </c>
       <c r="B12">
-        <v>1998</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>256</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>669</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>1101</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" t="s">
-        <v>785</v>
-      </c>
+        <v>2021</v>
+      </c>
+      <c r="C12" s="96" t="s">
+        <v>422</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>1625</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="I12" t="s">
-        <v>1521</v>
-      </c>
-      <c r="J12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" t="s">
-        <v>932</v>
-      </c>
-      <c r="M12" t="s">
-        <v>930</v>
+        <v>1629</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>931</v>
-      </c>
-      <c r="O12">
-        <v>44.512999999999998</v>
-      </c>
-      <c r="P12">
-        <v>-109.98</v>
-      </c>
-      <c r="Q12">
-        <v>4</v>
+        <v>1626</v>
+      </c>
+      <c r="O12" s="96">
+        <v>40.133513999999998</v>
+      </c>
+      <c r="P12" s="96">
+        <v>-111.771241</v>
+      </c>
+      <c r="Q12" s="96">
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="R12" t="s">
-        <v>933</v>
+        <v>1627</v>
       </c>
       <c r="S12" t="s">
         <v>22</v>
@@ -31378,32 +31382,13 @@
         <v>22</v>
       </c>
       <c r="U12" t="s">
-        <v>934</v>
+        <v>1628</v>
       </c>
       <c r="V12" t="s">
-        <v>1382</v>
-      </c>
-      <c r="W12" t="s">
-        <v>1422</v>
-      </c>
-      <c r="X12" t="s">
-        <v>1467</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>1468</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>1499</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>1156</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>1243</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>1243</v>
-      </c>
+        <v>1401</v>
+      </c>
+      <c r="Z12" s="116"/>
+      <c r="AA12" s="62"/>
       <c r="AE12" t="s">
         <v>1243</v>
       </c>
@@ -31412,53 +31397,86 @@
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>1595</v>
+      <c r="A13" s="125" t="s">
+        <v>928</v>
       </c>
       <c r="B13">
-        <v>1989</v>
+        <v>1998</v>
       </c>
       <c r="C13" t="s">
-        <v>1596</v>
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>256</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>785</v>
       </c>
       <c r="I13" t="s">
-        <v>1603</v>
+        <v>1521</v>
       </c>
       <c r="J13" t="s">
-        <v>1597</v>
+        <v>24</v>
       </c>
       <c r="K13" t="s">
-        <v>1598</v>
+        <v>932</v>
       </c>
       <c r="M13" t="s">
-        <v>1600</v>
+        <v>930</v>
       </c>
       <c r="N13" t="s">
-        <v>1599</v>
-      </c>
-      <c r="O13" s="94">
-        <v>49.704340000000002</v>
-      </c>
-      <c r="P13" s="94">
-        <v>-116.118877</v>
+        <v>931</v>
+      </c>
+      <c r="O13">
+        <v>44.512999999999998</v>
+      </c>
+      <c r="P13">
+        <v>-109.98</v>
       </c>
       <c r="Q13">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="R13" t="s">
+        <v>933</v>
+      </c>
+      <c r="S13" t="s">
+        <v>22</v>
       </c>
       <c r="T13" t="s">
         <v>22</v>
       </c>
       <c r="U13" t="s">
-        <v>1602</v>
+        <v>934</v>
       </c>
       <c r="V13" t="s">
-        <v>1401</v>
+        <v>1382</v>
       </c>
       <c r="W13" t="s">
         <v>1422</v>
       </c>
       <c r="X13" t="s">
-        <v>1601</v>
+        <v>1467</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>1468</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>1499</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>1156</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>1243</v>
       </c>
       <c r="AD13" t="s">
         <v>1243</v>
@@ -31471,43 +31489,53 @@
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>670</v>
+      <c r="A14" s="125" t="s">
+        <v>1595</v>
       </c>
       <c r="B14">
-        <v>2000</v>
+        <v>1989</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+        <v>1596</v>
+      </c>
       <c r="I14" t="s">
-        <v>1522</v>
+        <v>1603</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1597</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1598</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1600</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1599</v>
+      </c>
+      <c r="O14" s="94">
+        <v>49.704340000000002</v>
+      </c>
+      <c r="P14" s="94">
+        <v>-116.118877</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="T14" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" t="s">
+        <v>1602</v>
       </c>
       <c r="V14" t="s">
-        <v>1381</v>
+        <v>1401</v>
       </c>
       <c r="W14" t="s">
         <v>1422</v>
       </c>
       <c r="X14" t="s">
-        <v>1469</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>1470</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>1505</v>
-      </c>
-      <c r="AA14" s="114" t="s">
-        <v>1471</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>1156</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>1243</v>
+        <v>1601</v>
       </c>
       <c r="AD14" t="s">
         <v>1243</v>
@@ -31519,130 +31547,95 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>909</v>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A15" s="125" t="s">
+        <v>670</v>
       </c>
       <c r="B15">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="C15" t="s">
-        <v>246</v>
+        <v>73</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="I15" t="s">
-        <v>1511</v>
-      </c>
-      <c r="K15" s="97"/>
-      <c r="N15" s="98"/>
+        <v>1522</v>
+      </c>
       <c r="V15" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
       <c r="W15" t="s">
-        <v>1436</v>
+        <v>1422</v>
       </c>
       <c r="X15" t="s">
-        <v>1446</v>
-      </c>
-      <c r="Y15" s="96" t="s">
-        <v>1156</v>
-      </c>
-      <c r="Z15" s="96" t="s">
-        <v>1493</v>
+        <v>1469</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>1470</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>1505</v>
+      </c>
+      <c r="AA15" s="114" t="s">
+        <v>1471</v>
       </c>
       <c r="AB15" t="s">
         <v>1156</v>
       </c>
       <c r="AC15" t="s">
-        <v>1490</v>
+        <v>1243</v>
       </c>
       <c r="AD15" t="s">
-        <v>1615</v>
+        <v>1243</v>
       </c>
       <c r="AE15" t="s">
         <v>1243</v>
       </c>
-      <c r="AF15" t="s">
-        <v>1623</v>
-      </c>
       <c r="AG15" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="96" t="s">
-        <v>1183</v>
+      <c r="A16" s="125" t="s">
+        <v>909</v>
       </c>
       <c r="B16">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="C16" t="s">
-        <v>481</v>
-      </c>
-      <c r="D16" t="s">
-        <v>482</v>
-      </c>
-      <c r="E16" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" t="s">
-        <v>785</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
       <c r="I16" t="s">
-        <v>1531</v>
-      </c>
-      <c r="J16" t="s">
-        <v>1184</v>
+        <v>1511</v>
       </c>
       <c r="K16" s="97"/>
-      <c r="M16">
-        <v>4</v>
-      </c>
-      <c r="N16" s="98" t="s">
-        <v>1186</v>
-      </c>
-      <c r="O16">
-        <v>44.910800000000002</v>
-      </c>
-      <c r="P16">
-        <v>-116.1031</v>
-      </c>
-      <c r="S16" t="s">
-        <v>22</v>
-      </c>
-      <c r="U16" t="s">
-        <v>1185</v>
-      </c>
+      <c r="N16" s="98"/>
       <c r="V16" t="s">
-        <v>1401</v>
+        <v>1385</v>
       </c>
       <c r="W16" t="s">
-        <v>1422</v>
+        <v>1436</v>
       </c>
       <c r="X16" t="s">
-        <v>1418</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>1472</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>1506</v>
+        <v>1446</v>
+      </c>
+      <c r="Y16" s="96" t="s">
+        <v>1156</v>
+      </c>
+      <c r="Z16" s="96" t="s">
+        <v>1493</v>
       </c>
       <c r="AB16" t="s">
         <v>1156</v>
       </c>
       <c r="AC16" t="s">
-        <v>1484</v>
+        <v>1490</v>
       </c>
       <c r="AD16" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="AE16" t="s">
         <v>1243</v>
@@ -31654,18 +31647,18 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>727</v>
+    <row r="17" spans="1:33" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="125" t="s">
+        <v>1183</v>
       </c>
       <c r="B17">
-        <v>1998</v>
+        <v>2015</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>481</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>482</v>
       </c>
       <c r="E17" s="11" t="b">
         <v>1</v>
@@ -31680,87 +31673,82 @@
         <v>785</v>
       </c>
       <c r="I17" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
       <c r="J17" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" t="s">
-        <v>724</v>
-      </c>
-      <c r="L17" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" t="s">
-        <v>725</v>
-      </c>
-      <c r="O17" s="99">
-        <v>48.762999999999998</v>
-      </c>
-      <c r="P17" s="99">
-        <v>-114.226</v>
-      </c>
-      <c r="Q17" s="100">
-        <v>5</v>
-      </c>
-      <c r="R17" s="100" t="s">
-        <v>726</v>
-      </c>
-      <c r="T17" t="s">
+        <v>1184</v>
+      </c>
+      <c r="K17" s="97"/>
+      <c r="M17">
+        <v>4</v>
+      </c>
+      <c r="N17" s="98" t="s">
+        <v>1186</v>
+      </c>
+      <c r="O17">
+        <v>44.910800000000002</v>
+      </c>
+      <c r="P17">
+        <v>-116.1031</v>
+      </c>
+      <c r="S17" t="s">
         <v>22</v>
       </c>
       <c r="U17" t="s">
-        <v>1395</v>
+        <v>1185</v>
       </c>
       <c r="V17" t="s">
         <v>1401</v>
       </c>
       <c r="W17" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="X17" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="Y17" t="s">
-        <v>1156</v>
-      </c>
-      <c r="Z17" s="116" t="s">
-        <v>1497</v>
+        <v>1472</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>1506</v>
       </c>
       <c r="AB17" t="s">
         <v>1156</v>
       </c>
       <c r="AC17" t="s">
-        <v>1243</v>
+        <v>1484</v>
       </c>
       <c r="AD17" t="s">
-        <v>1243</v>
+        <v>1616</v>
       </c>
       <c r="AE17" t="s">
         <v>1243</v>
       </c>
+      <c r="AF17" t="s">
+        <v>1623</v>
+      </c>
       <c r="AG17" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>1165</v>
+      <c r="A18" s="125" t="s">
+        <v>727</v>
       </c>
       <c r="B18">
-        <v>2023</v>
+        <v>1998</v>
       </c>
       <c r="C18" t="s">
-        <v>470</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>471</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>669</v>
+        <v>108</v>
+      </c>
+      <c r="E18" s="11" t="b">
+        <v>1</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>1101</v>
+        <v>3</v>
       </c>
       <c r="G18" t="s">
         <v>17</v>
@@ -31769,52 +31757,52 @@
         <v>785</v>
       </c>
       <c r="I18" t="s">
-        <v>1514</v>
+        <v>1530</v>
       </c>
       <c r="J18" t="s">
-        <v>1168</v>
-      </c>
-      <c r="L18" s="46" t="s">
-        <v>1166</v>
-      </c>
-      <c r="M18" t="s">
-        <v>987</v>
+        <v>24</v>
+      </c>
+      <c r="K18" t="s">
+        <v>724</v>
+      </c>
+      <c r="L18" t="s">
+        <v>19</v>
       </c>
       <c r="N18" t="s">
-        <v>1167</v>
-      </c>
-      <c r="O18">
-        <v>38.916015999999999</v>
-      </c>
-      <c r="P18">
-        <v>-120.281718</v>
-      </c>
-      <c r="Q18">
-        <v>2</v>
-      </c>
-      <c r="R18" t="s">
-        <v>1170</v>
-      </c>
-      <c r="S18" t="s">
+        <v>725</v>
+      </c>
+      <c r="O18" s="99">
+        <v>48.762999999999998</v>
+      </c>
+      <c r="P18" s="99">
+        <v>-114.226</v>
+      </c>
+      <c r="Q18" s="100">
+        <v>5</v>
+      </c>
+      <c r="R18" s="100" t="s">
+        <v>726</v>
+      </c>
+      <c r="T18" t="s">
         <v>22</v>
       </c>
       <c r="U18" t="s">
-        <v>1169</v>
+        <v>1395</v>
       </c>
       <c r="V18" t="s">
-        <v>1382</v>
+        <v>1401</v>
       </c>
       <c r="W18" t="s">
         <v>1424</v>
       </c>
       <c r="X18" t="s">
-        <v>1434</v>
+        <v>1419</v>
       </c>
       <c r="Y18" t="s">
         <v>1156</v>
       </c>
       <c r="Z18" s="116" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="AB18" t="s">
         <v>1156</v>
@@ -31823,7 +31811,7 @@
         <v>1243</v>
       </c>
       <c r="AD18" t="s">
-        <v>1615</v>
+        <v>1243</v>
       </c>
       <c r="AE18" t="s">
         <v>1243</v>
@@ -31832,205 +31820,200 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>1231</v>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A19" s="125" t="s">
+        <v>1165</v>
       </c>
       <c r="B19">
-        <v>2016</v>
+        <v>2023</v>
       </c>
       <c r="C19" t="s">
-        <v>1447</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+        <v>470</v>
+      </c>
+      <c r="D19" t="s">
+        <v>471</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>785</v>
+      </c>
       <c r="I19" t="s">
-        <v>1510</v>
-      </c>
-      <c r="L19" s="46"/>
+        <v>1514</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1168</v>
+      </c>
+      <c r="L19" s="46" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M19" t="s">
+        <v>987</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1167</v>
+      </c>
+      <c r="O19">
+        <v>38.916015999999999</v>
+      </c>
+      <c r="P19">
+        <v>-120.281718</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19" t="s">
+        <v>1170</v>
+      </c>
+      <c r="S19" t="s">
+        <v>22</v>
+      </c>
+      <c r="U19" t="s">
+        <v>1169</v>
+      </c>
       <c r="V19" t="s">
-        <v>1390</v>
+        <v>1382</v>
       </c>
       <c r="W19" t="s">
-        <v>1430</v>
-      </c>
-      <c r="X19" s="112" t="s">
-        <v>1448</v>
-      </c>
-      <c r="Y19" s="96" t="s">
+        <v>1424</v>
+      </c>
+      <c r="X19" t="s">
+        <v>1434</v>
+      </c>
+      <c r="Y19" t="s">
         <v>1156</v>
       </c>
-      <c r="Z19" s="96" t="s">
-        <v>1492</v>
+      <c r="Z19" s="116" t="s">
+        <v>1499</v>
       </c>
       <c r="AB19" t="s">
         <v>1156</v>
       </c>
       <c r="AC19" t="s">
-        <v>1489</v>
+        <v>1243</v>
       </c>
       <c r="AD19" t="s">
-        <v>1243</v>
+        <v>1615</v>
       </c>
       <c r="AE19" t="s">
         <v>1243</v>
       </c>
-      <c r="AF19" t="s">
-        <v>1623</v>
-      </c>
       <c r="AG19" t="s">
-        <v>1624</v>
-      </c>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>1233</v>
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" ht="19" x14ac:dyDescent="0.2">
+      <c r="A20" s="125" t="s">
+        <v>1231</v>
       </c>
       <c r="B20">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="C20" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="I20" t="s">
-        <v>1509</v>
-      </c>
+        <v>1510</v>
+      </c>
+      <c r="L20" s="46"/>
       <c r="V20" t="s">
-        <v>1450</v>
+        <v>1390</v>
       </c>
       <c r="W20" t="s">
-        <v>1455</v>
-      </c>
-      <c r="X20" t="s">
-        <v>1454</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>1244</v>
+        <v>1430</v>
+      </c>
+      <c r="X20" s="112" t="s">
+        <v>1448</v>
+      </c>
+      <c r="Y20" s="96" t="s">
+        <v>1156</v>
+      </c>
+      <c r="Z20" s="96" t="s">
+        <v>1492</v>
       </c>
       <c r="AB20" t="s">
         <v>1156</v>
       </c>
       <c r="AC20" t="s">
+        <v>1489</v>
+      </c>
+      <c r="AD20" t="s">
         <v>1243</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>1617</v>
       </c>
       <c r="AE20" t="s">
         <v>1243</v>
       </c>
+      <c r="AF20" t="s">
+        <v>1623</v>
+      </c>
       <c r="AG20" t="s">
-        <v>1243</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A21" s="96" t="s">
-        <v>750</v>
-      </c>
-      <c r="B21" s="96">
-        <v>2008</v>
-      </c>
-      <c r="C21" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="96" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="101" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="93" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="102" t="s">
-        <v>785</v>
-      </c>
+      <c r="A21" s="125" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B21">
+        <v>2015</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1449</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
       <c r="I21" t="s">
-        <v>1523</v>
-      </c>
-      <c r="J21" s="93" t="s">
-        <v>751</v>
-      </c>
-      <c r="K21" s="93" t="s">
-        <v>752</v>
-      </c>
-      <c r="L21" s="93" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="96"/>
-      <c r="N21" s="93" t="s">
-        <v>753</v>
-      </c>
-      <c r="O21" s="94">
-        <v>48.789253000000002</v>
-      </c>
-      <c r="P21" s="94">
-        <v>-113.79626500000001</v>
-      </c>
-      <c r="Q21" s="95">
-        <v>4</v>
-      </c>
-      <c r="R21" s="95" t="s">
-        <v>754</v>
-      </c>
-      <c r="S21" s="96" t="s">
-        <v>22</v>
-      </c>
-      <c r="T21" s="96" t="s">
-        <v>22</v>
-      </c>
-      <c r="U21" s="96" t="s">
-        <v>1392</v>
-      </c>
-      <c r="V21" s="96" t="s">
-        <v>1403</v>
-      </c>
-      <c r="W21" s="96" t="s">
-        <v>1422</v>
-      </c>
-      <c r="X21" s="96" t="s">
-        <v>1473</v>
-      </c>
-      <c r="Y21" s="96" t="s">
-        <v>1474</v>
-      </c>
-      <c r="Z21" s="116" t="s">
-        <v>1507</v>
+        <v>1509</v>
+      </c>
+      <c r="V21" t="s">
+        <v>1450</v>
+      </c>
+      <c r="W21" t="s">
+        <v>1455</v>
+      </c>
+      <c r="X21" t="s">
+        <v>1454</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>1244</v>
       </c>
       <c r="AB21" t="s">
         <v>1156</v>
       </c>
       <c r="AC21" t="s">
-        <v>1485</v>
+        <v>1243</v>
       </c>
       <c r="AD21" t="s">
-        <v>1243</v>
+        <v>1617</v>
       </c>
       <c r="AE21" t="s">
         <v>1243</v>
       </c>
-      <c r="AF21" s="125"/>
-      <c r="AG21" s="125" t="s">
+      <c r="AG21" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A22" s="96" t="s">
-        <v>826</v>
+      <c r="A22" s="125" t="s">
+        <v>750</v>
       </c>
       <c r="B22" s="96">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="C22" s="96" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="96" t="s">
-        <v>184</v>
+        <v>125</v>
       </c>
       <c r="E22" s="101" t="b">
         <v>1</v>
@@ -32038,41 +32021,39 @@
       <c r="F22" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="96" t="s">
+      <c r="G22" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="96" t="s">
-        <v>693</v>
-      </c>
-      <c r="I22" s="96" t="s">
-        <v>1524</v>
+      <c r="H22" s="102" t="s">
+        <v>785</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1523</v>
       </c>
       <c r="J22" s="93" t="s">
-        <v>827</v>
+        <v>751</v>
       </c>
       <c r="K22" s="93" t="s">
-        <v>828</v>
+        <v>752</v>
       </c>
       <c r="L22" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="103" t="s">
-        <v>833</v>
-      </c>
+      <c r="M22" s="96"/>
       <c r="N22" s="93" t="s">
-        <v>829</v>
+        <v>753</v>
       </c>
       <c r="O22" s="94">
-        <v>40.353888888</v>
+        <v>48.789253000000002</v>
       </c>
       <c r="P22" s="94">
-        <v>-105.583611111</v>
+        <v>-113.79626500000001</v>
       </c>
       <c r="Q22" s="95">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R22" s="95" t="s">
-        <v>830</v>
+        <v>754</v>
       </c>
       <c r="S22" s="96" t="s">
         <v>22</v>
@@ -32081,31 +32062,31 @@
         <v>22</v>
       </c>
       <c r="U22" s="96" t="s">
-        <v>831</v>
-      </c>
-      <c r="V22" t="s">
-        <v>1405</v>
-      </c>
-      <c r="W22" t="s">
+        <v>1392</v>
+      </c>
+      <c r="V22" s="96" t="s">
+        <v>1403</v>
+      </c>
+      <c r="W22" s="96" t="s">
         <v>1422</v>
       </c>
-      <c r="X22" t="s">
-        <v>1423</v>
+      <c r="X22" s="96" t="s">
+        <v>1473</v>
       </c>
       <c r="Y22" s="96" t="s">
-        <v>1475</v>
-      </c>
-      <c r="Z22" s="96" t="s">
-        <v>1499</v>
+        <v>1474</v>
+      </c>
+      <c r="Z22" s="116" t="s">
+        <v>1507</v>
       </c>
       <c r="AB22" t="s">
         <v>1156</v>
       </c>
       <c r="AC22" t="s">
+        <v>1485</v>
+      </c>
+      <c r="AD22" t="s">
         <v>1243</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>1485</v>
       </c>
       <c r="AE22" t="s">
         <v>1243</v>
@@ -32115,73 +32096,84 @@
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>711</v>
-      </c>
-      <c r="B23">
-        <v>2015</v>
-      </c>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>669</v>
+      <c r="A23" s="125" t="s">
+        <v>826</v>
+      </c>
+      <c r="B23" s="96">
+        <v>2016</v>
+      </c>
+      <c r="C23" s="96" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="96" t="s">
+        <v>184</v>
+      </c>
+      <c r="E23" s="101" t="b">
+        <v>1</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>1101</v>
-      </c>
-      <c r="G23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="H23" t="s">
-        <v>785</v>
+      <c r="H23" s="96" t="s">
+        <v>693</v>
       </c>
       <c r="I23" s="96" t="s">
-        <v>1525</v>
-      </c>
-      <c r="L23" t="s">
+        <v>1524</v>
+      </c>
+      <c r="J23" s="93" t="s">
+        <v>827</v>
+      </c>
+      <c r="K23" s="93" t="s">
+        <v>828</v>
+      </c>
+      <c r="L23" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="N23" t="s">
-        <v>708</v>
-      </c>
-      <c r="O23">
-        <v>40.033332999999999</v>
-      </c>
-      <c r="P23">
-        <v>-105.416667</v>
-      </c>
-      <c r="Q23">
-        <v>3</v>
-      </c>
-      <c r="R23" t="s">
-        <v>709</v>
-      </c>
-      <c r="S23" t="s">
+      <c r="M23" s="103" t="s">
+        <v>833</v>
+      </c>
+      <c r="N23" s="93" t="s">
+        <v>829</v>
+      </c>
+      <c r="O23" s="94">
+        <v>40.353888888</v>
+      </c>
+      <c r="P23" s="94">
+        <v>-105.583611111</v>
+      </c>
+      <c r="Q23" s="95">
+        <v>2</v>
+      </c>
+      <c r="R23" s="95" t="s">
+        <v>830</v>
+      </c>
+      <c r="S23" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="T23" t="s">
+      <c r="T23" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="U23" t="s">
-        <v>710</v>
+      <c r="U23" s="96" t="s">
+        <v>831</v>
       </c>
       <c r="V23" t="s">
-        <v>1382</v>
+        <v>1405</v>
       </c>
       <c r="W23" t="s">
         <v>1422</v>
       </c>
       <c r="X23" t="s">
-        <v>1435</v>
+        <v>1423</v>
       </c>
       <c r="Y23" s="96" t="s">
-        <v>1476</v>
-      </c>
-      <c r="Z23" s="96"/>
+        <v>1475</v>
+      </c>
+      <c r="Z23" s="96" t="s">
+        <v>1499</v>
+      </c>
       <c r="AB23" t="s">
         <v>1156</v>
       </c>
@@ -32189,7 +32181,7 @@
         <v>1243</v>
       </c>
       <c r="AD23" t="s">
-        <v>1243</v>
+        <v>1485</v>
       </c>
       <c r="AE23" t="s">
         <v>1243</v>
@@ -32199,41 +32191,50 @@
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>848</v>
+      <c r="A24" s="125" t="s">
+        <v>711</v>
       </c>
       <c r="B24">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>198</v>
-      </c>
-      <c r="E24" s="11" t="b">
-        <v>1</v>
+        <v>96</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>669</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>3</v>
+        <v>1101</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="s">
+        <v>785</v>
       </c>
       <c r="I24" s="96" t="s">
         <v>1525</v>
       </c>
-      <c r="M24" t="s">
-        <v>849</v>
+      <c r="L24" t="s">
+        <v>19</v>
       </c>
       <c r="N24" t="s">
-        <v>1377</v>
+        <v>708</v>
       </c>
       <c r="O24">
-        <v>40.050263700000002</v>
+        <v>40.033332999999999</v>
       </c>
       <c r="P24">
-        <v>-105.3666599</v>
+        <v>-105.416667</v>
       </c>
       <c r="Q24">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="R24" t="s">
+        <v>709</v>
       </c>
       <c r="S24" t="s">
         <v>22</v>
@@ -32242,23 +32243,21 @@
         <v>22</v>
       </c>
       <c r="U24" t="s">
-        <v>850</v>
+        <v>710</v>
       </c>
       <c r="V24" t="s">
-        <v>1401</v>
+        <v>1382</v>
       </c>
       <c r="W24" t="s">
         <v>1422</v>
       </c>
       <c r="X24" t="s">
-        <v>1425</v>
+        <v>1435</v>
       </c>
       <c r="Y24" s="96" t="s">
         <v>1476</v>
       </c>
-      <c r="Z24" s="96" t="s">
-        <v>1499</v>
-      </c>
+      <c r="Z24" s="96"/>
       <c r="AB24" t="s">
         <v>1156</v>
       </c>
@@ -32276,162 +32275,159 @@
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>1605</v>
+      <c r="A25" s="125" t="s">
+        <v>848</v>
       </c>
       <c r="B25">
-        <v>1982</v>
+        <v>2018</v>
       </c>
       <c r="C25" t="s">
-        <v>1606</v>
-      </c>
-      <c r="I25" t="s">
-        <v>1607</v>
-      </c>
-      <c r="J25" t="s">
-        <v>1608</v>
-      </c>
-      <c r="K25" t="s">
-        <v>1609</v>
-      </c>
-      <c r="M25">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="11" t="b">
         <v>1</v>
       </c>
+      <c r="F25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="96" t="s">
+        <v>1525</v>
+      </c>
+      <c r="M25" t="s">
+        <v>849</v>
+      </c>
       <c r="N25" t="s">
-        <v>1610</v>
+        <v>1377</v>
       </c>
       <c r="O25">
-        <v>36.095348999999999</v>
+        <v>40.050263700000002</v>
       </c>
       <c r="P25">
-        <v>-82.265000000000001</v>
+        <v>-105.3666599</v>
       </c>
       <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="R25" t="s">
-        <v>989</v>
+        <v>5</v>
+      </c>
+      <c r="S25" t="s">
+        <v>22</v>
       </c>
       <c r="T25" t="s">
         <v>22</v>
       </c>
       <c r="U25" t="s">
-        <v>1611</v>
+        <v>850</v>
       </c>
       <c r="V25" t="s">
-        <v>1612</v>
+        <v>1401</v>
       </c>
       <c r="W25" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
       <c r="X25" t="s">
-        <v>1613</v>
+        <v>1425</v>
+      </c>
+      <c r="Y25" s="96" t="s">
+        <v>1476</v>
+      </c>
+      <c r="Z25" s="96" t="s">
+        <v>1499</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>1156</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>1243</v>
       </c>
       <c r="AD25" t="s">
         <v>1243</v>
       </c>
+      <c r="AE25" t="s">
+        <v>1243</v>
+      </c>
       <c r="AG25" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>881</v>
+      <c r="A26" s="125" t="s">
+        <v>1605</v>
       </c>
       <c r="B26">
-        <v>2012</v>
+        <v>1982</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" t="s">
-        <v>223</v>
-      </c>
-      <c r="E26" s="11" t="b">
+        <v>1606</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1607</v>
+      </c>
+      <c r="J26" t="s">
+        <v>1608</v>
+      </c>
+      <c r="K26" t="s">
+        <v>1609</v>
+      </c>
+      <c r="M26">
         <v>1</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" t="s">
-        <v>785</v>
-      </c>
-      <c r="I26" t="s">
-        <v>1515</v>
-      </c>
-      <c r="J26" t="s">
-        <v>882</v>
-      </c>
-      <c r="M26" t="s">
-        <v>883</v>
-      </c>
       <c r="N26" t="s">
-        <v>884</v>
+        <v>1610</v>
       </c>
       <c r="O26">
-        <v>38.896382000000003</v>
+        <v>36.095348999999999</v>
       </c>
       <c r="P26">
-        <v>-120.041629</v>
+        <v>-82.265000000000001</v>
       </c>
       <c r="Q26">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="R26" t="s">
+        <v>989</v>
       </c>
       <c r="T26" t="s">
         <v>22</v>
       </c>
       <c r="U26" t="s">
-        <v>887</v>
+        <v>1611</v>
       </c>
       <c r="V26" t="s">
-        <v>1401</v>
+        <v>1612</v>
       </c>
       <c r="W26" t="s">
-        <v>1424</v>
+        <v>1426</v>
       </c>
       <c r="X26" t="s">
-        <v>1498</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>1457</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>1156</v>
-      </c>
-      <c r="AC26" t="s">
-        <v>1243</v>
+        <v>1613</v>
       </c>
       <c r="AD26" t="s">
         <v>1243</v>
       </c>
-      <c r="AE26" t="s">
-        <v>1243</v>
-      </c>
       <c r="AG26" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>1091</v>
+      <c r="A27" s="125" t="s">
+        <v>881</v>
       </c>
       <c r="B27">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="C27" t="s">
-        <v>412</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>413</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>669</v>
+        <v>223</v>
+      </c>
+      <c r="E27" s="11" t="b">
+        <v>1</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>1101</v>
+        <v>3</v>
       </c>
       <c r="G27" t="s">
         <v>17</v>
@@ -32440,55 +32436,49 @@
         <v>785</v>
       </c>
       <c r="I27" t="s">
-        <v>1527</v>
+        <v>1515</v>
       </c>
       <c r="J27" t="s">
-        <v>24</v>
-      </c>
-      <c r="K27" t="s">
-        <v>1094</v>
-      </c>
-      <c r="L27" t="s">
-        <v>1092</v>
+        <v>882</v>
       </c>
       <c r="M27" t="s">
-        <v>1093</v>
+        <v>883</v>
       </c>
       <c r="N27" t="s">
-        <v>1096</v>
+        <v>884</v>
       </c>
       <c r="O27">
-        <v>40.262369999999997</v>
+        <v>38.896382000000003</v>
       </c>
       <c r="P27">
-        <v>-105.59080400000001</v>
-      </c>
-      <c r="Q27" s="100">
-        <v>8.3000000000000004E-2</v>
+        <v>-120.041629</v>
+      </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
+      <c r="T27" t="s">
+        <v>22</v>
       </c>
       <c r="U27" t="s">
-        <v>1095</v>
+        <v>887</v>
       </c>
       <c r="V27" t="s">
-        <v>1382</v>
+        <v>1401</v>
       </c>
       <c r="W27" t="s">
-        <v>1436</v>
+        <v>1424</v>
       </c>
       <c r="X27" t="s">
-        <v>1437</v>
-      </c>
-      <c r="Y27" s="96" t="s">
-        <v>1156</v>
-      </c>
-      <c r="Z27" s="96" t="s">
-        <v>1493</v>
+        <v>1498</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>1457</v>
       </c>
       <c r="AB27" t="s">
         <v>1156</v>
       </c>
       <c r="AC27" t="s">
-        <v>1490</v>
+        <v>1243</v>
       </c>
       <c r="AD27" t="s">
         <v>1243</v>
@@ -32496,23 +32486,22 @@
       <c r="AE27" t="s">
         <v>1243</v>
       </c>
-      <c r="AF27" s="125"/>
-      <c r="AG27" s="125" t="s">
+      <c r="AG27" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>689</v>
+      <c r="A28" s="125" t="s">
+        <v>1091</v>
       </c>
       <c r="B28">
-        <v>2011</v>
+        <v>2021</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>412</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>413</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>669</v>
@@ -32524,85 +32513,81 @@
         <v>17</v>
       </c>
       <c r="H28" t="s">
-        <v>693</v>
+        <v>785</v>
       </c>
       <c r="I28" t="s">
-        <v>1511</v>
+        <v>1527</v>
       </c>
       <c r="J28" t="s">
         <v>24</v>
       </c>
       <c r="K28" t="s">
-        <v>694</v>
+        <v>1094</v>
       </c>
       <c r="L28" t="s">
-        <v>19</v>
+        <v>1092</v>
+      </c>
+      <c r="M28" t="s">
+        <v>1093</v>
       </c>
       <c r="N28" t="s">
-        <v>695</v>
+        <v>1096</v>
       </c>
       <c r="O28">
-        <v>39.177683000000002</v>
+        <v>40.262369999999997</v>
       </c>
       <c r="P28">
-        <v>-105.26552</v>
-      </c>
-      <c r="Q28">
-        <v>5</v>
-      </c>
-      <c r="R28" t="s">
-        <v>690</v>
-      </c>
-      <c r="T28" t="s">
-        <v>22</v>
+        <v>-105.59080400000001</v>
+      </c>
+      <c r="Q28" s="100">
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="U28" t="s">
-        <v>696</v>
+        <v>1095</v>
       </c>
       <c r="V28" t="s">
         <v>1382</v>
       </c>
       <c r="W28" t="s">
-        <v>1439</v>
+        <v>1436</v>
       </c>
       <c r="X28" t="s">
-        <v>1438</v>
-      </c>
-      <c r="Y28" t="s">
+        <v>1437</v>
+      </c>
+      <c r="Y28" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z28" s="115" t="s">
+      <c r="Z28" s="96" t="s">
         <v>1493</v>
       </c>
       <c r="AB28" t="s">
         <v>1156</v>
       </c>
       <c r="AC28" t="s">
-        <v>1244</v>
+        <v>1490</v>
       </c>
       <c r="AD28" t="s">
-        <v>1618</v>
+        <v>1243</v>
       </c>
       <c r="AE28" t="s">
         <v>1243</v>
       </c>
-      <c r="AF28" s="125"/>
-      <c r="AG28" s="125" t="s">
+      <c r="AG28" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>762</v>
+      <c r="A29" s="125" t="s">
+        <v>689</v>
       </c>
       <c r="B29">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="C29" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>669</v>
@@ -32613,8 +32598,8 @@
       <c r="G29" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="102" t="s">
-        <v>785</v>
+      <c r="H29" t="s">
+        <v>693</v>
       </c>
       <c r="I29" t="s">
         <v>1511</v>
@@ -32629,7 +32614,7 @@
         <v>19</v>
       </c>
       <c r="N29" t="s">
-        <v>721</v>
+        <v>695</v>
       </c>
       <c r="O29">
         <v>39.177683000000002</v>
@@ -32637,38 +32622,41 @@
       <c r="P29">
         <v>-105.26552</v>
       </c>
-      <c r="S29" t="s">
-        <v>22</v>
+      <c r="Q29">
+        <v>5</v>
+      </c>
+      <c r="R29" t="s">
+        <v>690</v>
       </c>
       <c r="T29" t="s">
         <v>22</v>
       </c>
       <c r="U29" t="s">
-        <v>1108</v>
+        <v>696</v>
       </c>
       <c r="V29" t="s">
         <v>1382</v>
       </c>
       <c r="W29" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="X29" t="s">
-        <v>1441</v>
+        <v>1438</v>
       </c>
       <c r="Y29" t="s">
         <v>1156</v>
       </c>
-      <c r="Z29" t="s">
-        <v>1494</v>
+      <c r="Z29" s="115" t="s">
+        <v>1493</v>
       </c>
       <c r="AB29" t="s">
         <v>1156</v>
       </c>
       <c r="AC29" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="AD29" t="s">
-        <v>1243</v>
+        <v>1618</v>
       </c>
       <c r="AE29" t="s">
         <v>1243</v>
@@ -32678,47 +32666,50 @@
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>924</v>
+      <c r="A30" s="125" t="s">
+        <v>762</v>
       </c>
       <c r="B30">
         <v>2019</v>
       </c>
       <c r="C30" t="s">
-        <v>254</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E30" s="11" t="b">
-        <v>1</v>
+        <v>127</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>669</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>3</v>
+        <v>1101</v>
       </c>
       <c r="G30" t="s">
         <v>17</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="102" t="s">
         <v>785</v>
       </c>
       <c r="I30" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="J30" t="s">
-        <v>873</v>
-      </c>
-      <c r="M30" t="s">
-        <v>926</v>
+        <v>24</v>
+      </c>
+      <c r="K30" t="s">
+        <v>694</v>
+      </c>
+      <c r="L30" t="s">
+        <v>19</v>
       </c>
       <c r="N30" t="s">
-        <v>927</v>
+        <v>721</v>
       </c>
       <c r="O30">
-        <v>37.534036999999998</v>
+        <v>39.177683000000002</v>
       </c>
       <c r="P30">
-        <v>-119.389139</v>
+        <v>-105.26552</v>
       </c>
       <c r="S30" t="s">
         <v>22</v>
@@ -32727,90 +32718,93 @@
         <v>22</v>
       </c>
       <c r="U30" t="s">
-        <v>925</v>
+        <v>1108</v>
       </c>
       <c r="V30" t="s">
-        <v>1401</v>
+        <v>1382</v>
       </c>
       <c r="W30" t="s">
-        <v>1426</v>
+        <v>1440</v>
       </c>
       <c r="X30" t="s">
-        <v>1427</v>
+        <v>1441</v>
       </c>
       <c r="Y30" t="s">
         <v>1156</v>
       </c>
-      <c r="Z30" s="116" t="s">
-        <v>1495</v>
+      <c r="Z30" t="s">
+        <v>1494</v>
       </c>
       <c r="AB30" t="s">
         <v>1156</v>
       </c>
       <c r="AC30" t="s">
-        <v>1483</v>
+        <v>1243</v>
       </c>
       <c r="AD30" t="s">
-        <v>1619</v>
+        <v>1243</v>
       </c>
       <c r="AE30" t="s">
         <v>1243</v>
       </c>
-      <c r="AF30" t="s">
-        <v>1623</v>
-      </c>
       <c r="AG30" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>948</v>
+      <c r="A31" s="125" t="s">
+        <v>924</v>
       </c>
       <c r="B31">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="C31" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D31" t="s">
-        <v>268</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>669</v>
+        <v>255</v>
+      </c>
+      <c r="E31" s="11" t="b">
+        <v>1</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>1101</v>
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>17</v>
       </c>
       <c r="H31" t="s">
         <v>785</v>
       </c>
       <c r="I31" t="s">
-        <v>1528</v>
+        <v>1513</v>
+      </c>
+      <c r="J31" t="s">
+        <v>873</v>
       </c>
       <c r="M31" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="N31" t="s">
-        <v>949</v>
+        <v>927</v>
       </c>
       <c r="O31">
-        <v>44.578524999999999</v>
+        <v>37.534036999999998</v>
       </c>
       <c r="P31">
-        <v>-115.66604</v>
-      </c>
-      <c r="Q31">
-        <v>4</v>
+        <v>-119.389139</v>
+      </c>
+      <c r="S31" t="s">
+        <v>22</v>
       </c>
       <c r="T31" t="s">
         <v>22</v>
       </c>
       <c r="U31" t="s">
-        <v>950</v>
+        <v>925</v>
       </c>
       <c r="V31" t="s">
-        <v>1386</v>
+        <v>1401</v>
       </c>
       <c r="W31" t="s">
         <v>1426</v>
@@ -32822,81 +32816,93 @@
         <v>1156</v>
       </c>
       <c r="Z31" s="116" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="AB31" t="s">
         <v>1156</v>
       </c>
       <c r="AC31" t="s">
-        <v>1244</v>
+        <v>1483</v>
       </c>
       <c r="AD31" t="s">
-        <v>1243</v>
+        <v>1619</v>
       </c>
       <c r="AE31" t="s">
         <v>1243</v>
       </c>
-      <c r="AF31" s="8" t="s">
-        <v>1488</v>
-      </c>
-      <c r="AG31" s="8" t="s">
+      <c r="AF31" t="s">
+        <v>1623</v>
+      </c>
+      <c r="AG31" t="s">
         <v>1244</v>
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A32" s="93" t="s">
-        <v>1586</v>
+      <c r="A32" s="125" t="s">
+        <v>948</v>
       </c>
       <c r="B32">
-        <v>1973</v>
+        <v>2015</v>
       </c>
       <c r="C32" t="s">
-        <v>1587</v>
+        <v>267</v>
+      </c>
+      <c r="D32" t="s">
+        <v>268</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H32" t="s">
+        <v>785</v>
       </c>
       <c r="I32" t="s">
-        <v>1588</v>
-      </c>
-      <c r="J32" t="s">
-        <v>24</v>
-      </c>
-      <c r="K32" t="s">
-        <v>1589</v>
-      </c>
-      <c r="L32" t="s">
-        <v>19</v>
+        <v>1528</v>
       </c>
       <c r="M32" t="s">
-        <v>883</v>
+        <v>930</v>
       </c>
       <c r="N32" t="s">
-        <v>1590</v>
-      </c>
-      <c r="O32" s="122">
-        <v>48.102674999999998</v>
-      </c>
-      <c r="P32" s="122">
-        <v>-120.35232000000001</v>
+        <v>949</v>
+      </c>
+      <c r="O32">
+        <v>44.578524999999999</v>
+      </c>
+      <c r="P32">
+        <v>-115.66604</v>
       </c>
       <c r="Q32">
-        <v>2</v>
-      </c>
-      <c r="R32" t="s">
-        <v>1591</v>
+        <v>4</v>
       </c>
       <c r="T32" t="s">
         <v>22</v>
       </c>
       <c r="U32" t="s">
-        <v>1592</v>
+        <v>950</v>
       </c>
       <c r="V32" t="s">
-        <v>1401</v>
+        <v>1386</v>
       </c>
       <c r="W32" t="s">
         <v>1426</v>
       </c>
       <c r="X32" t="s">
-        <v>1593</v>
+        <v>1427</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>1156</v>
+      </c>
+      <c r="Z32" s="116" t="s">
+        <v>1496</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>1156</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>1244</v>
       </c>
       <c r="AD32" t="s">
         <v>1243</v>
@@ -32904,116 +32910,96 @@
       <c r="AE32" t="s">
         <v>1243</v>
       </c>
-      <c r="AG32" t="s">
-        <v>1243</v>
+      <c r="AF32" s="8" t="s">
+        <v>1488</v>
+      </c>
+      <c r="AG32" s="8" t="s">
+        <v>1244</v>
       </c>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>871</v>
+      <c r="A33" s="125" t="s">
+        <v>1586</v>
       </c>
       <c r="B33">
-        <v>2020</v>
+        <v>1973</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" t="s">
-        <v>219</v>
-      </c>
-      <c r="E33" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" t="s">
-        <v>785</v>
-      </c>
-      <c r="I33" s="96" t="s">
-        <v>1526</v>
+        <v>1587</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1588</v>
       </c>
       <c r="J33" t="s">
-        <v>873</v>
-      </c>
-      <c r="M33" s="104" t="s">
-        <v>874</v>
+        <v>24</v>
+      </c>
+      <c r="K33" t="s">
+        <v>1589</v>
+      </c>
+      <c r="L33" t="s">
+        <v>19</v>
+      </c>
+      <c r="M33" t="s">
+        <v>883</v>
       </c>
       <c r="N33" t="s">
-        <v>875</v>
-      </c>
-      <c r="O33">
-        <v>38.512031</v>
-      </c>
-      <c r="P33">
-        <v>-122.097228</v>
+        <v>1590</v>
+      </c>
+      <c r="O33" s="122">
+        <v>48.102674999999998</v>
+      </c>
+      <c r="P33" s="122">
+        <v>-120.35232000000001</v>
       </c>
       <c r="Q33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R33" t="s">
-        <v>876</v>
-      </c>
-      <c r="S33" t="s">
-        <v>22</v>
+        <v>1591</v>
       </c>
       <c r="T33" t="s">
         <v>22</v>
       </c>
       <c r="U33" t="s">
-        <v>872</v>
+        <v>1592</v>
       </c>
       <c r="V33" t="s">
         <v>1401</v>
       </c>
       <c r="W33" t="s">
-        <v>1422</v>
+        <v>1426</v>
       </c>
       <c r="X33" t="s">
-        <v>1428</v>
-      </c>
-      <c r="Y33" s="96" t="s">
-        <v>1477</v>
-      </c>
-      <c r="Z33" s="96"/>
-      <c r="AB33" t="s">
-        <v>1156</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>1487</v>
+        <v>1593</v>
       </c>
       <c r="AD33" t="s">
-        <v>1485</v>
+        <v>1243</v>
       </c>
       <c r="AE33" t="s">
         <v>1243</v>
       </c>
-      <c r="AF33" s="125"/>
-      <c r="AG33" s="125" t="s">
+      <c r="AG33" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>765</v>
+      <c r="A34" s="125" t="s">
+        <v>871</v>
       </c>
       <c r="B34">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>669</v>
+        <v>219</v>
+      </c>
+      <c r="E34" s="11" t="b">
+        <v>1</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>1101</v>
+        <v>3</v>
       </c>
       <c r="G34" t="s">
         <v>17</v>
@@ -33021,65 +33007,60 @@
       <c r="H34" t="s">
         <v>785</v>
       </c>
-      <c r="I34" t="s">
-        <v>1512</v>
-      </c>
-      <c r="J34" s="108" t="s">
-        <v>770</v>
-      </c>
-      <c r="K34" s="108" t="s">
-        <v>771</v>
-      </c>
-      <c r="L34" s="108" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34">
-        <v>1</v>
-      </c>
-      <c r="N34" s="108" t="s">
-        <v>767</v>
-      </c>
-      <c r="O34" s="109">
-        <v>40.7159999</v>
-      </c>
-      <c r="P34" s="109">
-        <v>-105.23308400000001</v>
-      </c>
-      <c r="Q34" s="110">
-        <v>0.5</v>
-      </c>
-      <c r="R34" s="110" t="s">
-        <v>768</v>
+      <c r="I34" s="96" t="s">
+        <v>1526</v>
+      </c>
+      <c r="J34" t="s">
+        <v>873</v>
+      </c>
+      <c r="M34" s="104" t="s">
+        <v>874</v>
+      </c>
+      <c r="N34" t="s">
+        <v>875</v>
+      </c>
+      <c r="O34">
+        <v>38.512031</v>
+      </c>
+      <c r="P34">
+        <v>-122.097228</v>
+      </c>
+      <c r="Q34">
+        <v>3</v>
+      </c>
+      <c r="R34" t="s">
+        <v>876</v>
       </c>
       <c r="S34" t="s">
         <v>22</v>
       </c>
+      <c r="T34" t="s">
+        <v>22</v>
+      </c>
       <c r="U34" t="s">
-        <v>769</v>
+        <v>872</v>
       </c>
       <c r="V34" t="s">
-        <v>1382</v>
+        <v>1401</v>
       </c>
       <c r="W34" t="s">
-        <v>1430</v>
+        <v>1422</v>
       </c>
       <c r="X34" t="s">
-        <v>1442</v>
+        <v>1428</v>
       </c>
       <c r="Y34" s="96" t="s">
-        <v>1156</v>
-      </c>
-      <c r="Z34" s="96" t="s">
-        <v>1492</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="Z34" s="96"/>
       <c r="AB34" t="s">
         <v>1156</v>
       </c>
       <c r="AC34" t="s">
-        <v>1243</v>
+        <v>1487</v>
       </c>
       <c r="AD34" t="s">
-        <v>1243</v>
+        <v>1485</v>
       </c>
       <c r="AE34" t="s">
         <v>1243</v>
@@ -33089,152 +33070,247 @@
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>1232</v>
+      <c r="A35" s="125" t="s">
+        <v>765</v>
       </c>
       <c r="B35">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="C35" t="s">
-        <v>1451</v>
-      </c>
-      <c r="I35" s="96" t="s">
-        <v>1525</v>
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" t="s">
+        <v>785</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1512</v>
+      </c>
+      <c r="J35" s="108" t="s">
+        <v>770</v>
+      </c>
+      <c r="K35" s="108" t="s">
+        <v>771</v>
+      </c>
+      <c r="L35" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35" s="108" t="s">
+        <v>767</v>
+      </c>
+      <c r="O35" s="109">
+        <v>40.7159999</v>
+      </c>
+      <c r="P35" s="109">
+        <v>-105.23308400000001</v>
+      </c>
+      <c r="Q35" s="110">
+        <v>0.5</v>
+      </c>
+      <c r="R35" s="110" t="s">
+        <v>768</v>
+      </c>
+      <c r="S35" t="s">
+        <v>22</v>
+      </c>
+      <c r="U35" t="s">
+        <v>769</v>
+      </c>
+      <c r="V35" t="s">
+        <v>1382</v>
       </c>
       <c r="W35" t="s">
-        <v>1422</v>
+        <v>1430</v>
       </c>
       <c r="X35" t="s">
-        <v>1452</v>
+        <v>1442</v>
       </c>
       <c r="Y35" s="96" t="s">
-        <v>1478</v>
-      </c>
-      <c r="Z35" s="96"/>
+        <v>1156</v>
+      </c>
+      <c r="Z35" s="96" t="s">
+        <v>1492</v>
+      </c>
       <c r="AB35" t="s">
         <v>1156</v>
       </c>
       <c r="AC35" t="s">
-        <v>1488</v>
+        <v>1243</v>
       </c>
       <c r="AD35" t="s">
-        <v>1620</v>
+        <v>1243</v>
       </c>
       <c r="AE35" t="s">
         <v>1243</v>
       </c>
-      <c r="AF35" s="8" t="s">
-        <v>1488</v>
-      </c>
-      <c r="AG35" s="8" t="s">
-        <v>1244</v>
+      <c r="AG35" t="s">
+        <v>1243</v>
       </c>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>789</v>
+      <c r="A36" s="125" t="s">
+        <v>1232</v>
       </c>
       <c r="B36">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
-      </c>
-      <c r="D36" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H36" t="s">
-        <v>785</v>
-      </c>
-      <c r="I36" t="s">
-        <v>1510</v>
-      </c>
-      <c r="J36" s="96" t="s">
-        <v>770</v>
-      </c>
-      <c r="K36" s="96" t="s">
-        <v>771</v>
-      </c>
-      <c r="L36" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" s="96"/>
-      <c r="N36" s="96" t="s">
-        <v>767</v>
-      </c>
-      <c r="O36">
-        <v>40.702464999999997</v>
-      </c>
-      <c r="P36">
-        <v>-105.241646</v>
-      </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-      <c r="R36" t="s">
-        <v>790</v>
-      </c>
-      <c r="S36" t="s">
-        <v>22</v>
-      </c>
-      <c r="T36" t="s">
-        <v>22</v>
-      </c>
-      <c r="U36" t="s">
-        <v>791</v>
-      </c>
-      <c r="V36" t="s">
-        <v>1401</v>
+        <v>1451</v>
+      </c>
+      <c r="I36" s="96" t="s">
+        <v>1525</v>
       </c>
       <c r="W36" t="s">
-        <v>1430</v>
+        <v>1422</v>
       </c>
       <c r="X36" t="s">
-        <v>1429</v>
+        <v>1452</v>
       </c>
       <c r="Y36" s="96" t="s">
-        <v>1156</v>
-      </c>
-      <c r="Z36" s="96" t="s">
-        <v>1492</v>
-      </c>
+        <v>1478</v>
+      </c>
+      <c r="Z36" s="96"/>
       <c r="AB36" t="s">
         <v>1156</v>
       </c>
       <c r="AC36" t="s">
-        <v>1243</v>
+        <v>1488</v>
       </c>
       <c r="AD36" t="s">
-        <v>1243</v>
+        <v>1620</v>
       </c>
       <c r="AE36" t="s">
         <v>1243</v>
       </c>
-      <c r="AG36" t="s">
+      <c r="AF36" s="8" t="s">
+        <v>1488</v>
+      </c>
+      <c r="AG36" s="8" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A37" s="125" t="s">
+        <v>789</v>
+      </c>
+      <c r="B37">
+        <v>2014</v>
+      </c>
+      <c r="C37" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H37" t="s">
+        <v>785</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1510</v>
+      </c>
+      <c r="J37" s="96" t="s">
+        <v>770</v>
+      </c>
+      <c r="K37" s="96" t="s">
+        <v>771</v>
+      </c>
+      <c r="L37" s="96" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="96"/>
+      <c r="N37" s="96" t="s">
+        <v>767</v>
+      </c>
+      <c r="O37">
+        <v>40.702464999999997</v>
+      </c>
+      <c r="P37">
+        <v>-105.241646</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+      <c r="R37" t="s">
+        <v>790</v>
+      </c>
+      <c r="S37" t="s">
+        <v>22</v>
+      </c>
+      <c r="T37" t="s">
+        <v>22</v>
+      </c>
+      <c r="U37" t="s">
+        <v>791</v>
+      </c>
+      <c r="V37" t="s">
+        <v>1401</v>
+      </c>
+      <c r="W37" t="s">
+        <v>1430</v>
+      </c>
+      <c r="X37" t="s">
+        <v>1429</v>
+      </c>
+      <c r="Y37" s="96" t="s">
+        <v>1156</v>
+      </c>
+      <c r="Z37" s="96" t="s">
+        <v>1492</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>1156</v>
+      </c>
+      <c r="AC37" t="s">
         <v>1243</v>
       </c>
+      <c r="AD37" t="s">
+        <v>1243</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>1243</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>1243</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD36">
-    <sortCondition ref="B2:B36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD37">
+    <sortCondition ref="B2:B37"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7 F19:F24" xr:uid="{8B21EFF3-D61C-024F-A87C-4FC0F83918E4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7 F20:F25" xr:uid="{8B21EFF3-D61C-024F-A87C-4FC0F83918E4}">
       <formula1>"No fire event, no DOC/NO3, No river, Prescribed Burn, Maybe"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F27:F32 F8:F18" xr:uid="{0E623121-76BB-5545-A51E-3CA5AE425338}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28:F33 F8:F19" xr:uid="{0E623121-76BB-5545-A51E-3CA5AE425338}">
       <formula1>"Included, No fire event, no DOC/NO3, No river, Prescribed Burn, Wrong study design, Maybe"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25:F26" xr:uid="{6293A447-FF72-D446-A29F-02B4F97196AE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26:F27" xr:uid="{6293A447-FF72-D446-A29F-02B4F97196AE}">
       <formula1>"No fire event, no DOC/NO3, No river, Prescribed Burn, Wrong study design, Maybe"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D12" r:id="rId1" xr:uid="{73D7F5F8-4377-1E4E-A0CC-C0B3159C0DFF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating lat/longs for HUCs
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
+++ b/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF0C57F-330D-5F42-8D71-3E5FEF7AF934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D62C4F3-B747-A646-906B-C3BA65E8AF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="4" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
+    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="4" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
   </bookViews>
   <sheets>
     <sheet name="Study_info" sheetId="2" r:id="rId1"/>
@@ -30422,7 +30422,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <selection pane="topRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Building effect size models
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
+++ b/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A529F-4BB7-4C4F-BB8F-F979306F8BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8A380D-1AE4-3A43-A06B-254C7CDA8663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="4" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6741" uniqueCount="1630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6746" uniqueCount="1634">
   <si>
     <t>Study</t>
   </si>
@@ -4721,69 +4721,12 @@
     <t>Hewlett Gulch_High Park fire</t>
   </si>
   <si>
-    <t>Hayman Fire (2002)</t>
-  </si>
-  <si>
-    <t>High Park Fire (2012)</t>
-  </si>
-  <si>
     <t>Yosemite NP Fire</t>
   </si>
   <si>
-    <t>Angora Fire (2007)</t>
-  </si>
-  <si>
-    <t>Anaktuvuk River wildfire (2007)</t>
-  </si>
-  <si>
-    <t>Thompson Ridge Wildfire (2013)</t>
-  </si>
-  <si>
-    <t>Boundary Fire (2004)</t>
-  </si>
-  <si>
-    <t>Lost Creek Wildfire (2003)</t>
-  </si>
-  <si>
-    <t>Camp Branch Fire (2016)_Tellico Fire (2016)</t>
-  </si>
-  <si>
-    <t>Clover-Mist Wildfire (1988)</t>
-  </si>
-  <si>
     <t>Historic Fires</t>
   </si>
   <si>
-    <t>Rampage Fire (2003)_Others in Glacier NP</t>
-  </si>
-  <si>
-    <t>Fern Lake (2012)</t>
-  </si>
-  <si>
-    <t>Fourmile Canyon Fire (2010)</t>
-  </si>
-  <si>
-    <t>Rocky Fire (2015)_Wragg Fire (2015)</t>
-  </si>
-  <si>
-    <t>Hayman Fire (2002)_High Park Fire (2012)</t>
-  </si>
-  <si>
-    <t>No name given (2002)</t>
-  </si>
-  <si>
-    <t>Northwest Territories Fire (2013)</t>
-  </si>
-  <si>
-    <t>Red Bench Fire (1988)</t>
-  </si>
-  <si>
-    <t>No name given (2007)</t>
-  </si>
-  <si>
-    <t>Gaviota Fire (2004)</t>
-  </si>
-  <si>
     <t>My_Search</t>
   </si>
   <si>
@@ -4949,9 +4892,6 @@
     <t>Stream chemistry following a forest fire and urea fertilization in north-central Washington</t>
   </si>
   <si>
-    <t>Safety Harbor Fire (1970)</t>
-  </si>
-  <si>
     <t>Ponderosa pine, bitterbrush, bluebunch wheatgrass, cheatgrass, arrowleaf balsamroot, Douglas fir, Pinegrass, Ross sedge, alder, willow, subalpine fir, whitebark pine</t>
   </si>
   <si>
@@ -4994,9 +4934,6 @@
     <t xml:space="preserve">Figure 3 has nitrate-N for East fork (burned) middle fork (burned) and West Fork (unburned). Hampton has already extracted this data and Ill be using that </t>
   </si>
   <si>
-    <t>Matt fire, 1985</t>
-  </si>
-  <si>
     <t>added</t>
   </si>
   <si>
@@ -5072,10 +5009,85 @@
     <t>Can only find TOC data to extract or take from the supplemental</t>
   </si>
   <si>
-    <t>Pole Creek Fire Complex (2018)</t>
-  </si>
-  <si>
-    <t>Caldor Fire(2021)_Mosquito Fire (2022)</t>
+    <t>Fire_year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anaktuvuk River wildfire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thompson Ridge Wildfire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boundary Fire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost Creek Wildfire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northwest Territories Fire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camp Branch Fire_Tellico Fire </t>
+  </si>
+  <si>
+    <t>2021_2022</t>
+  </si>
+  <si>
+    <t>2002_2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaviota Fire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pole Creek Fire Complex </t>
+  </si>
+  <si>
+    <t>Clover-Mist Wildfire</t>
+  </si>
+  <si>
+    <t>Matt fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hayman Fire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No name given </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Bench Fire </t>
+  </si>
+  <si>
+    <t>Caldor Fire_Mosquito Fire</t>
+  </si>
+  <si>
+    <t>Rampage Fire_Others in Glacier NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fern Lake </t>
+  </si>
+  <si>
+    <t>Fourmile Canyon Fire</t>
+  </si>
+  <si>
+    <t>Angora Fire</t>
+  </si>
+  <si>
+    <t>Hayman Fire_High Park Fire</t>
+  </si>
+  <si>
+    <t>No name given</t>
+  </si>
+  <si>
+    <t>Safety Harbor Fire</t>
+  </si>
+  <si>
+    <t>Rocky Fire_Wragg Fire</t>
+  </si>
+  <si>
+    <t>High Park Fire</t>
+  </si>
+  <si>
+    <t>2012_2012</t>
   </si>
 </sst>
 </file>
@@ -30418,11 +30430,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E83DAFB-3D69-1A4C-8997-3EF8B4236F27}">
-  <dimension ref="A1:AG37"/>
+  <dimension ref="A1:AH37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I36" sqref="I36"/>
+      <selection pane="topRight" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30431,15 +30443,16 @@
     <col min="2" max="2" width="9.1640625" customWidth="1"/>
     <col min="5" max="8" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="22" width="10.83203125" customWidth="1"/>
-    <col min="23" max="23" width="9.6640625" customWidth="1"/>
-    <col min="24" max="24" width="37.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.5" customWidth="1"/>
-    <col min="31" max="31" width="4" customWidth="1"/>
-    <col min="32" max="32" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="38.6640625" customWidth="1"/>
+    <col min="11" max="23" width="10.83203125" customWidth="1"/>
+    <col min="24" max="24" width="9.6640625" customWidth="1"/>
+    <col min="25" max="25" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.5" customWidth="1"/>
+    <col min="32" max="32" width="4" customWidth="1"/>
+    <col min="33" max="33" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -30468,79 +30481,82 @@
         <v>1508</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>1607</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="74" t="s">
+      <c r="W1" s="74" t="s">
         <v>1380</v>
       </c>
-      <c r="W1" s="105" t="s">
+      <c r="X1" s="105" t="s">
         <v>1421</v>
       </c>
-      <c r="X1" s="105" t="s">
+      <c r="Y1" s="105" t="s">
         <v>1420</v>
       </c>
-      <c r="Y1" s="105" t="s">
+      <c r="Z1" s="105" t="s">
         <v>1456</v>
       </c>
-      <c r="Z1" s="105" t="s">
+      <c r="AA1" s="105" t="s">
         <v>1491</v>
       </c>
-      <c r="AA1" s="105" t="s">
+      <c r="AB1" s="105" t="s">
         <v>1464</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>1479</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>1486</v>
       </c>
-      <c r="AD1" s="105" t="s">
-        <v>1613</v>
-      </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="105" t="s">
+        <v>1592</v>
+      </c>
+      <c r="AF1" s="6" t="s">
         <v>1379</v>
       </c>
-      <c r="AF1" s="6" t="s">
-        <v>1620</v>
-      </c>
       <c r="AG1" s="6" t="s">
-        <v>1621</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+        <v>1599</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="125" t="s">
         <v>935</v>
       </c>
@@ -30566,49 +30582,49 @@
         <v>785</v>
       </c>
       <c r="I2" t="s">
-        <v>1515</v>
-      </c>
-      <c r="M2" t="s">
+        <v>1608</v>
+      </c>
+      <c r="J2">
+        <v>2007</v>
+      </c>
+      <c r="N2" t="s">
         <v>937</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>938</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>69.166667000000004</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>-150.75</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>2</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>22</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>939</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>1382</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>1432</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>1431</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>1458</v>
       </c>
-      <c r="Z2" s="116" t="s">
+      <c r="AA2" s="116" t="s">
         <v>1499</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>1481</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>1243</v>
       </c>
       <c r="AD2" t="s">
         <v>1243</v>
@@ -30616,11 +30632,14 @@
       <c r="AE2" t="s">
         <v>1243</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AF2" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH2" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="125" t="s">
         <v>1174</v>
       </c>
@@ -30646,70 +30665,73 @@
         <v>692</v>
       </c>
       <c r="I3" s="106" t="s">
-        <v>1516</v>
-      </c>
-      <c r="L3" t="s">
+        <v>1609</v>
+      </c>
+      <c r="J3" s="106">
+        <v>2013</v>
+      </c>
+      <c r="M3" t="s">
         <v>1176</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>1177</v>
       </c>
-      <c r="N3" s="106" t="s">
+      <c r="O3" s="106" t="s">
         <v>1175</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>35.890813000000001</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>-106.540854</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>9</v>
-      </c>
-      <c r="S3" t="s">
-        <v>22</v>
       </c>
       <c r="T3" t="s">
         <v>22</v>
       </c>
       <c r="U3" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" t="s">
         <v>1178</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>1390</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>1422</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>1433</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>1463</v>
       </c>
-      <c r="Z3" s="116" t="s">
+      <c r="AA3" s="116" t="s">
         <v>1499</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>1480</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>1483</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>1243</v>
       </c>
       <c r="AE3" t="s">
         <v>1243</v>
       </c>
       <c r="AF3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="AG3" t="s">
         <v>1488</v>
       </c>
-      <c r="AG3" t="s">
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH3" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="125" t="s">
         <v>681</v>
       </c>
@@ -30736,25 +30758,23 @@
       <c r="L4" s="60"/>
       <c r="M4" s="60"/>
       <c r="N4" s="60"/>
-      <c r="P4" s="60"/>
+      <c r="O4" s="60"/>
       <c r="Q4" s="60"/>
       <c r="R4" s="60"/>
       <c r="S4" s="60"/>
       <c r="T4" s="60"/>
-      <c r="U4" s="60" t="s">
+      <c r="U4" s="60"/>
+      <c r="V4" s="60" t="s">
         <v>682</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>1406</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>1156</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>1243</v>
       </c>
       <c r="AD4" t="s">
         <v>1243</v>
@@ -30762,11 +30782,14 @@
       <c r="AE4" t="s">
         <v>1243</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AF4" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH4" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="125" t="s">
         <v>681</v>
       </c>
@@ -30794,56 +30817,53 @@
       <c r="I5" t="s">
         <v>1156</v>
       </c>
-      <c r="J5" s="93" t="s">
+      <c r="K5" s="93" t="s">
         <v>733</v>
       </c>
-      <c r="K5" s="93" t="s">
+      <c r="L5" s="93" t="s">
         <v>734</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="93" t="s">
+      <c r="O5" s="93" t="s">
         <v>731</v>
       </c>
-      <c r="O5" s="94">
+      <c r="P5" s="94">
         <v>49.667000000000002</v>
       </c>
-      <c r="P5" s="94">
+      <c r="Q5" s="94">
         <v>-93.733000000000004</v>
       </c>
-      <c r="Q5" s="95">
+      <c r="R5" s="95">
         <v>15</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>732</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>22</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>1394</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>1390</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>1422</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>1414</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>1244</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>1499</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>1243</v>
       </c>
       <c r="AD5" t="s">
         <v>1243</v>
@@ -30851,14 +30871,17 @@
       <c r="AE5" t="s">
         <v>1243</v>
       </c>
-      <c r="AF5" s="124" t="s">
+      <c r="AF5" t="s">
+        <v>1243</v>
+      </c>
+      <c r="AG5" s="124" t="s">
         <v>1488</v>
       </c>
-      <c r="AG5" s="124" t="s">
+      <c r="AH5" s="124" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="125" t="s">
         <v>1404</v>
       </c>
@@ -30884,70 +30907,73 @@
         <v>693</v>
       </c>
       <c r="I6" t="s">
-        <v>1517</v>
-      </c>
-      <c r="L6" t="s">
+        <v>1610</v>
+      </c>
+      <c r="J6">
+        <v>2004</v>
+      </c>
+      <c r="M6" t="s">
         <v>19</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>784</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>783</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>65.150000000000006</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>-147.5</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>3</v>
-      </c>
-      <c r="S6" t="s">
-        <v>22</v>
       </c>
       <c r="T6" t="s">
         <v>22</v>
       </c>
       <c r="U6" t="s">
+        <v>22</v>
+      </c>
+      <c r="V6" t="s">
         <v>782</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>1405</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>1422</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>1415</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>1459</v>
       </c>
-      <c r="Z6" s="116" t="s">
+      <c r="AA6" s="116" t="s">
         <v>1500</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>1156</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>1483</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>1243</v>
       </c>
       <c r="AE6" t="s">
         <v>1243</v>
       </c>
       <c r="AF6" t="s">
-        <v>1622</v>
+        <v>1243</v>
       </c>
       <c r="AG6" t="s">
+        <v>1601</v>
+      </c>
+      <c r="AH6" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="125" t="s">
         <v>1413</v>
       </c>
@@ -30973,70 +30999,73 @@
         <v>785</v>
       </c>
       <c r="I7" t="s">
-        <v>1518</v>
-      </c>
-      <c r="J7" t="s">
+        <v>1611</v>
+      </c>
+      <c r="J7">
+        <v>2003</v>
+      </c>
+      <c r="K7" t="s">
         <v>24</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>741</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>19</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>742</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>49.616667</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>-114.666667</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>3</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>744</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>22</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>1393</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>1401</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>1422</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>1416</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>1460</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>1501</v>
       </c>
-      <c r="AB7" s="114" t="s">
+      <c r="AC7" s="114" t="s">
         <v>1156</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>1243</v>
       </c>
-      <c r="AD7" t="s">
-        <v>1615</v>
-      </c>
       <c r="AE7" t="s">
+        <v>1594</v>
+      </c>
+      <c r="AF7" t="s">
         <v>1243</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="125" t="s">
         <v>835</v>
       </c>
@@ -31062,64 +31091,67 @@
         <v>785</v>
       </c>
       <c r="I8" t="s">
-        <v>1528</v>
-      </c>
-      <c r="M8">
+        <v>1612</v>
+      </c>
+      <c r="J8">
+        <v>2013</v>
+      </c>
+      <c r="N8">
         <v>3</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>836</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>61.4</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>-121.433333</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>0.5</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>743</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>22</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>837</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>1382</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>1424</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>1453</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>1156</v>
       </c>
-      <c r="Z8" s="116" t="s">
+      <c r="AA8" s="116" t="s">
         <v>1499</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>1156</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>1243</v>
       </c>
       <c r="AE8" t="s">
         <v>1243</v>
       </c>
       <c r="AF8" t="s">
+        <v>1243</v>
+      </c>
+      <c r="AG8" t="s">
         <v>1487</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AH8" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="125" t="s">
         <v>1001</v>
       </c>
@@ -31142,73 +31174,76 @@
         <v>785</v>
       </c>
       <c r="I9" t="s">
-        <v>1519</v>
-      </c>
-      <c r="J9" t="s">
+        <v>1613</v>
+      </c>
+      <c r="J9">
+        <v>2016</v>
+      </c>
+      <c r="K9" t="s">
         <v>1004</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>1002</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>1378</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>35</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>-83</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>2</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>989</v>
-      </c>
-      <c r="S9" t="s">
-        <v>22</v>
       </c>
       <c r="T9" t="s">
         <v>22</v>
       </c>
       <c r="U9" t="s">
+        <v>22</v>
+      </c>
+      <c r="V9" t="s">
         <v>1005</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>1382</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>1422</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>1502</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>1461</v>
       </c>
-      <c r="Z9" s="116" t="s">
+      <c r="AA9" s="116" t="s">
         <v>1503</v>
       </c>
-      <c r="AB9" s="113" t="s">
+      <c r="AC9" s="113" t="s">
         <v>1156</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>1483</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>1243</v>
       </c>
       <c r="AE9" t="s">
         <v>1243</v>
       </c>
-      <c r="AF9" s="8" t="s">
+      <c r="AF9" t="s">
+        <v>1243</v>
+      </c>
+      <c r="AG9" s="8" t="s">
         <v>1488</v>
       </c>
-      <c r="AG9" s="8" t="s">
+      <c r="AH9" s="8" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="125" t="s">
         <v>982</v>
       </c>
@@ -31231,67 +31266,70 @@
         <v>785</v>
       </c>
       <c r="I10" t="s">
-        <v>1511</v>
-      </c>
-      <c r="M10" t="s">
+        <v>695</v>
+      </c>
+      <c r="J10">
+        <v>2002</v>
+      </c>
+      <c r="N10" t="s">
         <v>985</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>695</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>39.177683000000002</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>-105.26552</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>2</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>984</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>22</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>983</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>1401</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>1422</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>1417</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>1462</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>1499</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>1482</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>1483</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>1243</v>
       </c>
       <c r="AE10" t="s">
         <v>1243</v>
       </c>
       <c r="AF10" t="s">
-        <v>1622</v>
+        <v>1243</v>
       </c>
       <c r="AG10" t="s">
+        <v>1601</v>
+      </c>
+      <c r="AH10" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="125" t="s">
         <v>1443</v>
       </c>
@@ -31304,31 +31342,31 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="I11" t="s">
-        <v>1531</v>
-      </c>
-      <c r="V11" t="s">
+        <v>1616</v>
+      </c>
+      <c r="J11">
+        <v>2004</v>
+      </c>
+      <c r="W11" t="s">
         <v>1401</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>1422</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>1445</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>1465</v>
       </c>
-      <c r="Z11" s="116" t="s">
+      <c r="AA11" s="116" t="s">
         <v>1504</v>
       </c>
-      <c r="AA11" s="62" t="s">
+      <c r="AB11" s="62" t="s">
         <v>1466</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>1243</v>
       </c>
       <c r="AD11" t="s">
         <v>1243</v>
@@ -31336,11 +31374,14 @@
       <c r="AE11" t="s">
         <v>1243</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AF11" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH11" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="125" t="s">
         <v>1115</v>
       </c>
@@ -31351,53 +31392,56 @@
         <v>422</v>
       </c>
       <c r="D12" s="62" t="s">
-        <v>1624</v>
+        <v>1603</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="I12" t="s">
-        <v>1628</v>
-      </c>
-      <c r="M12">
+        <v>1617</v>
+      </c>
+      <c r="J12">
+        <v>2018</v>
+      </c>
+      <c r="N12">
         <v>0</v>
       </c>
-      <c r="N12" t="s">
-        <v>1625</v>
-      </c>
-      <c r="O12" s="96">
+      <c r="O12" t="s">
+        <v>1604</v>
+      </c>
+      <c r="P12" s="96">
         <v>40.133513999999998</v>
       </c>
-      <c r="P12" s="96">
+      <c r="Q12" s="96">
         <v>-111.771241</v>
       </c>
-      <c r="Q12" s="96">
+      <c r="R12" s="96">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="R12" t="s">
-        <v>1626</v>
-      </c>
       <c r="S12" t="s">
-        <v>22</v>
+        <v>1605</v>
       </c>
       <c r="T12" t="s">
         <v>22</v>
       </c>
       <c r="U12" t="s">
-        <v>1627</v>
+        <v>22</v>
       </c>
       <c r="V12" t="s">
+        <v>1606</v>
+      </c>
+      <c r="W12" t="s">
         <v>1401</v>
       </c>
-      <c r="Z12" s="116"/>
-      <c r="AA12" s="62"/>
-      <c r="AE12" t="s">
+      <c r="AA12" s="116"/>
+      <c r="AB12" s="62"/>
+      <c r="AF12" t="s">
         <v>1243</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AH12" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="125" t="s">
         <v>928</v>
       </c>
@@ -31423,61 +31467,61 @@
         <v>785</v>
       </c>
       <c r="I13" t="s">
-        <v>1520</v>
-      </c>
-      <c r="J13" t="s">
+        <v>1618</v>
+      </c>
+      <c r="J13">
+        <v>1988</v>
+      </c>
+      <c r="K13" t="s">
         <v>24</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>932</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>930</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>931</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>44.512999999999998</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>-109.98</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>4</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>933</v>
-      </c>
-      <c r="S13" t="s">
-        <v>22</v>
       </c>
       <c r="T13" t="s">
         <v>22</v>
       </c>
       <c r="U13" t="s">
+        <v>22</v>
+      </c>
+      <c r="V13" t="s">
         <v>934</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>1382</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>1422</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>1467</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>1468</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AA13" t="s">
         <v>1499</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>1243</v>
       </c>
       <c r="AD13" t="s">
         <v>1243</v>
@@ -31485,70 +31529,76 @@
       <c r="AE13" t="s">
         <v>1243</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AF13" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH13" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="125" t="s">
-        <v>1594</v>
+        <v>1574</v>
       </c>
       <c r="B14">
         <v>1989</v>
       </c>
       <c r="C14" t="s">
-        <v>1595</v>
+        <v>1575</v>
       </c>
       <c r="I14" t="s">
-        <v>1602</v>
-      </c>
-      <c r="J14" t="s">
-        <v>1596</v>
+        <v>1619</v>
+      </c>
+      <c r="J14">
+        <v>1985</v>
       </c>
       <c r="K14" t="s">
-        <v>1597</v>
-      </c>
-      <c r="M14" t="s">
-        <v>1599</v>
+        <v>1576</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1577</v>
       </c>
       <c r="N14" t="s">
-        <v>1598</v>
-      </c>
-      <c r="O14" s="94">
+        <v>1579</v>
+      </c>
+      <c r="O14" t="s">
+        <v>1578</v>
+      </c>
+      <c r="P14" s="94">
         <v>49.704340000000002</v>
       </c>
-      <c r="P14" s="94">
+      <c r="Q14" s="94">
         <v>-116.118877</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>3</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>22</v>
       </c>
-      <c r="U14" t="s">
-        <v>1601</v>
-      </c>
       <c r="V14" t="s">
+        <v>1581</v>
+      </c>
+      <c r="W14" t="s">
         <v>1401</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>1422</v>
       </c>
-      <c r="X14" t="s">
-        <v>1600</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>1243</v>
+      <c r="Y14" t="s">
+        <v>1580</v>
       </c>
       <c r="AE14" t="s">
         <v>1243</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AF14" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH14" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="125" t="s">
         <v>670</v>
       </c>
@@ -31561,31 +31611,28 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="I15" t="s">
-        <v>1521</v>
-      </c>
-      <c r="V15" t="s">
+        <v>1512</v>
+      </c>
+      <c r="W15" t="s">
         <v>1381</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>1422</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>1469</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>1470</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>1505</v>
       </c>
-      <c r="AA15" s="114" t="s">
+      <c r="AB15" s="114" t="s">
         <v>1471</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>1243</v>
       </c>
       <c r="AD15" t="s">
         <v>1243</v>
@@ -31593,11 +31640,14 @@
       <c r="AE15" t="s">
         <v>1243</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AF15" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" ht="18" x14ac:dyDescent="0.2">
+      <c r="AH15" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="125" t="s">
         <v>909</v>
       </c>
@@ -31610,45 +31660,48 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="I16" t="s">
-        <v>1511</v>
-      </c>
-      <c r="K16" s="97"/>
-      <c r="N16" s="98"/>
-      <c r="V16" t="s">
+        <v>1620</v>
+      </c>
+      <c r="J16">
+        <v>2002</v>
+      </c>
+      <c r="L16" s="97"/>
+      <c r="O16" s="98"/>
+      <c r="W16" t="s">
         <v>1385</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>1436</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>1446</v>
       </c>
-      <c r="Y16" s="96" t="s">
+      <c r="Z16" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z16" s="96" t="s">
+      <c r="AA16" s="96" t="s">
         <v>1493</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AC16" t="s">
         <v>1156</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AD16" t="s">
         <v>1490</v>
       </c>
-      <c r="AD16" t="s">
-        <v>1614</v>
-      </c>
       <c r="AE16" t="s">
+        <v>1593</v>
+      </c>
+      <c r="AF16" t="s">
         <v>1243</v>
       </c>
-      <c r="AF16" t="s">
-        <v>1622</v>
-      </c>
       <c r="AG16" t="s">
+        <v>1601</v>
+      </c>
+      <c r="AH16" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="125" t="s">
         <v>1183</v>
       </c>
@@ -31674,65 +31727,68 @@
         <v>785</v>
       </c>
       <c r="I17" t="s">
-        <v>1530</v>
-      </c>
-      <c r="J17" t="s">
+        <v>1621</v>
+      </c>
+      <c r="J17">
+        <v>2007</v>
+      </c>
+      <c r="K17" t="s">
         <v>1184</v>
       </c>
-      <c r="K17" s="97"/>
-      <c r="M17">
+      <c r="L17" s="97"/>
+      <c r="N17">
         <v>4</v>
       </c>
-      <c r="N17" s="98" t="s">
+      <c r="O17" s="98" t="s">
         <v>1186</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>44.910800000000002</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>-116.1031</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>22</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>1185</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>1401</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>1422</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>1418</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>1472</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>1506</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AC17" t="s">
         <v>1156</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AD17" t="s">
         <v>1484</v>
       </c>
-      <c r="AD17" t="s">
-        <v>1615</v>
-      </c>
       <c r="AE17" t="s">
+        <v>1594</v>
+      </c>
+      <c r="AF17" t="s">
         <v>1243</v>
       </c>
-      <c r="AF17" t="s">
-        <v>1622</v>
-      </c>
       <c r="AG17" t="s">
+        <v>1601</v>
+      </c>
+      <c r="AH17" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="125" t="s">
         <v>727</v>
       </c>
@@ -31758,58 +31814,58 @@
         <v>785</v>
       </c>
       <c r="I18" t="s">
-        <v>1529</v>
-      </c>
-      <c r="J18" t="s">
+        <v>1622</v>
+      </c>
+      <c r="J18">
+        <v>1988</v>
+      </c>
+      <c r="K18" t="s">
         <v>24</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>724</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>19</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>725</v>
       </c>
-      <c r="O18" s="99">
+      <c r="P18" s="99">
         <v>48.762999999999998</v>
       </c>
-      <c r="P18" s="99">
+      <c r="Q18" s="99">
         <v>-114.226</v>
       </c>
-      <c r="Q18" s="100">
+      <c r="R18" s="100">
         <v>5</v>
       </c>
-      <c r="R18" s="100" t="s">
+      <c r="S18" s="100" t="s">
         <v>726</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>22</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>1395</v>
       </c>
-      <c r="V18" t="s">
+      <c r="W18" t="s">
         <v>1401</v>
       </c>
-      <c r="W18" t="s">
+      <c r="X18" t="s">
         <v>1424</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>1419</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>1156</v>
       </c>
-      <c r="Z18" s="116" t="s">
+      <c r="AA18" s="116" t="s">
         <v>1497</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AC18" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>1243</v>
       </c>
       <c r="AD18" t="s">
         <v>1243</v>
@@ -31817,11 +31873,14 @@
       <c r="AE18" t="s">
         <v>1243</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AF18" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH18" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="125" t="s">
         <v>1165</v>
       </c>
@@ -31847,70 +31906,73 @@
         <v>785</v>
       </c>
       <c r="I19" t="s">
-        <v>1629</v>
+        <v>1623</v>
       </c>
       <c r="J19" t="s">
+        <v>1614</v>
+      </c>
+      <c r="K19" t="s">
         <v>1168</v>
       </c>
-      <c r="L19" s="46" t="s">
+      <c r="M19" s="46" t="s">
         <v>1166</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>987</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>1167</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>38.916015999999999</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>-120.281718</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>2</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>1170</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>22</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>1169</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>1382</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>1424</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>1434</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>1156</v>
       </c>
-      <c r="Z19" s="116" t="s">
+      <c r="AA19" s="116" t="s">
         <v>1499</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AC19" t="s">
         <v>1156</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="AD19" t="s">
         <v>1243</v>
       </c>
-      <c r="AD19" t="s">
-        <v>1614</v>
-      </c>
       <c r="AE19" t="s">
+        <v>1593</v>
+      </c>
+      <c r="AF19" t="s">
         <v>1243</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AH19" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="125" t="s">
         <v>1231</v>
       </c>
@@ -31925,42 +31987,45 @@
       <c r="I20" t="s">
         <v>1510</v>
       </c>
-      <c r="L20" s="46"/>
-      <c r="V20" t="s">
+      <c r="J20" t="s">
+        <v>1633</v>
+      </c>
+      <c r="M20" s="46"/>
+      <c r="W20" t="s">
         <v>1390</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>1430</v>
       </c>
-      <c r="X20" s="112" t="s">
+      <c r="Y20" s="112" t="s">
         <v>1448</v>
       </c>
-      <c r="Y20" s="96" t="s">
+      <c r="Z20" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z20" s="96" t="s">
+      <c r="AA20" s="96" t="s">
         <v>1492</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AC20" t="s">
         <v>1156</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="AD20" t="s">
         <v>1489</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>1243</v>
       </c>
       <c r="AE20" t="s">
         <v>1243</v>
       </c>
       <c r="AF20" t="s">
-        <v>1622</v>
+        <v>1243</v>
       </c>
       <c r="AG20" t="s">
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+        <v>1601</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="125" t="s">
         <v>1233</v>
       </c>
@@ -31975,35 +32040,35 @@
       <c r="I21" t="s">
         <v>1509</v>
       </c>
-      <c r="V21" t="s">
+      <c r="W21" t="s">
         <v>1450</v>
       </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
         <v>1455</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>1454</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>1244</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AC21" t="s">
         <v>1156</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="AD21" t="s">
         <v>1243</v>
       </c>
-      <c r="AD21" t="s">
-        <v>1616</v>
-      </c>
       <c r="AE21" t="s">
+        <v>1595</v>
+      </c>
+      <c r="AF21" t="s">
         <v>1243</v>
       </c>
-      <c r="AG21" t="s">
+      <c r="AH21" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="125" t="s">
         <v>750</v>
       </c>
@@ -32029,74 +32094,77 @@
         <v>785</v>
       </c>
       <c r="I22" t="s">
-        <v>1522</v>
-      </c>
-      <c r="J22" s="93" t="s">
+        <v>1624</v>
+      </c>
+      <c r="J22">
+        <v>2003</v>
+      </c>
+      <c r="K22" s="93" t="s">
         <v>751</v>
       </c>
-      <c r="K22" s="93" t="s">
+      <c r="L22" s="93" t="s">
         <v>752</v>
       </c>
-      <c r="L22" s="93" t="s">
+      <c r="M22" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="96"/>
-      <c r="N22" s="93" t="s">
+      <c r="N22" s="96"/>
+      <c r="O22" s="93" t="s">
         <v>753</v>
       </c>
-      <c r="O22" s="94">
+      <c r="P22" s="94">
         <v>48.789253000000002</v>
       </c>
-      <c r="P22" s="94">
+      <c r="Q22" s="94">
         <v>-113.79626500000001</v>
       </c>
-      <c r="Q22" s="95">
+      <c r="R22" s="95">
         <v>4</v>
       </c>
-      <c r="R22" s="95" t="s">
+      <c r="S22" s="95" t="s">
         <v>754</v>
-      </c>
-      <c r="S22" s="96" t="s">
-        <v>22</v>
       </c>
       <c r="T22" s="96" t="s">
         <v>22</v>
       </c>
       <c r="U22" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="V22" s="96" t="s">
         <v>1392</v>
       </c>
-      <c r="V22" s="96" t="s">
+      <c r="W22" s="96" t="s">
         <v>1403</v>
       </c>
-      <c r="W22" s="96" t="s">
+      <c r="X22" s="96" t="s">
         <v>1422</v>
       </c>
-      <c r="X22" s="96" t="s">
+      <c r="Y22" s="96" t="s">
         <v>1473</v>
       </c>
-      <c r="Y22" s="96" t="s">
+      <c r="Z22" s="96" t="s">
         <v>1474</v>
       </c>
-      <c r="Z22" s="116" t="s">
+      <c r="AA22" s="116" t="s">
         <v>1507</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AC22" t="s">
         <v>1156</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AD22" t="s">
         <v>1485</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>1243</v>
       </c>
       <c r="AE22" t="s">
         <v>1243</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AF22" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH22" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="125" t="s">
         <v>826</v>
       </c>
@@ -32122,76 +32190,79 @@
         <v>693</v>
       </c>
       <c r="I23" s="96" t="s">
-        <v>1523</v>
-      </c>
-      <c r="J23" s="93" t="s">
+        <v>1625</v>
+      </c>
+      <c r="J23" s="96">
+        <v>2012</v>
+      </c>
+      <c r="K23" s="93" t="s">
         <v>827</v>
       </c>
-      <c r="K23" s="93" t="s">
+      <c r="L23" s="93" t="s">
         <v>828</v>
       </c>
-      <c r="L23" s="93" t="s">
+      <c r="M23" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="M23" s="103" t="s">
+      <c r="N23" s="103" t="s">
         <v>833</v>
       </c>
-      <c r="N23" s="93" t="s">
+      <c r="O23" s="93" t="s">
         <v>829</v>
       </c>
-      <c r="O23" s="94">
+      <c r="P23" s="94">
         <v>40.353888888</v>
       </c>
-      <c r="P23" s="94">
+      <c r="Q23" s="94">
         <v>-105.583611111</v>
       </c>
-      <c r="Q23" s="95">
+      <c r="R23" s="95">
         <v>2</v>
       </c>
-      <c r="R23" s="95" t="s">
+      <c r="S23" s="95" t="s">
         <v>830</v>
-      </c>
-      <c r="S23" s="96" t="s">
-        <v>22</v>
       </c>
       <c r="T23" s="96" t="s">
         <v>22</v>
       </c>
       <c r="U23" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="V23" s="96" t="s">
         <v>831</v>
       </c>
-      <c r="V23" t="s">
+      <c r="W23" t="s">
         <v>1405</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>1422</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>1423</v>
       </c>
-      <c r="Y23" s="96" t="s">
+      <c r="Z23" s="96" t="s">
         <v>1475</v>
       </c>
-      <c r="Z23" s="96" t="s">
+      <c r="AA23" s="96" t="s">
         <v>1499</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AC23" t="s">
         <v>1156</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="AD23" t="s">
         <v>1243</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AE23" t="s">
         <v>1485</v>
       </c>
-      <c r="AE23" t="s">
+      <c r="AF23" t="s">
         <v>1243</v>
       </c>
-      <c r="AG23" t="s">
+      <c r="AH23" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="125" t="s">
         <v>711</v>
       </c>
@@ -32217,53 +32288,53 @@
         <v>785</v>
       </c>
       <c r="I24" s="96" t="s">
-        <v>1524</v>
-      </c>
-      <c r="L24" t="s">
+        <v>1626</v>
+      </c>
+      <c r="J24" s="96">
+        <v>2010</v>
+      </c>
+      <c r="M24" t="s">
         <v>19</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>708</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>40.033332999999999</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>-105.416667</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>3</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>709</v>
-      </c>
-      <c r="S24" t="s">
-        <v>22</v>
       </c>
       <c r="T24" t="s">
         <v>22</v>
       </c>
       <c r="U24" t="s">
+        <v>22</v>
+      </c>
+      <c r="V24" t="s">
         <v>710</v>
       </c>
-      <c r="V24" t="s">
+      <c r="W24" t="s">
         <v>1382</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>1422</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" t="s">
         <v>1435</v>
       </c>
-      <c r="Y24" s="96" t="s">
+      <c r="Z24" s="96" t="s">
         <v>1476</v>
       </c>
-      <c r="Z24" s="96"/>
-      <c r="AB24" t="s">
+      <c r="AA24" s="96"/>
+      <c r="AC24" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>1243</v>
       </c>
       <c r="AD24" t="s">
         <v>1243</v>
@@ -32271,11 +32342,14 @@
       <c r="AE24" t="s">
         <v>1243</v>
       </c>
-      <c r="AG24" t="s">
+      <c r="AF24" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH24" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="125" t="s">
         <v>848</v>
       </c>
@@ -32295,52 +32369,52 @@
         <v>3</v>
       </c>
       <c r="I25" s="96" t="s">
-        <v>1524</v>
-      </c>
-      <c r="M25" t="s">
+        <v>1626</v>
+      </c>
+      <c r="J25" s="96">
+        <v>2010</v>
+      </c>
+      <c r="N25" t="s">
         <v>849</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>1377</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>40.050263700000002</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>-105.3666599</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>5</v>
-      </c>
-      <c r="S25" t="s">
-        <v>22</v>
       </c>
       <c r="T25" t="s">
         <v>22</v>
       </c>
       <c r="U25" t="s">
+        <v>22</v>
+      </c>
+      <c r="V25" t="s">
         <v>850</v>
       </c>
-      <c r="V25" t="s">
+      <c r="W25" t="s">
         <v>1401</v>
       </c>
-      <c r="W25" t="s">
+      <c r="X25" t="s">
         <v>1422</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" t="s">
         <v>1425</v>
       </c>
-      <c r="Y25" s="96" t="s">
+      <c r="Z25" s="96" t="s">
         <v>1476</v>
       </c>
-      <c r="Z25" s="96" t="s">
+      <c r="AA25" s="96" t="s">
         <v>1499</v>
       </c>
-      <c r="AB25" t="s">
+      <c r="AC25" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>1243</v>
       </c>
       <c r="AD25" t="s">
         <v>1243</v>
@@ -32348,70 +32422,73 @@
       <c r="AE25" t="s">
         <v>1243</v>
       </c>
-      <c r="AG25" t="s">
+      <c r="AF25" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH25" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="125" t="s">
-        <v>1604</v>
+        <v>1583</v>
       </c>
       <c r="B26">
         <v>1982</v>
       </c>
       <c r="C26" t="s">
-        <v>1605</v>
+        <v>1584</v>
       </c>
       <c r="I26" t="s">
-        <v>1606</v>
-      </c>
-      <c r="J26" t="s">
-        <v>1607</v>
+        <v>1585</v>
       </c>
       <c r="K26" t="s">
-        <v>1608</v>
-      </c>
-      <c r="M26">
+        <v>1586</v>
+      </c>
+      <c r="L26" t="s">
+        <v>1587</v>
+      </c>
+      <c r="N26">
         <v>1</v>
       </c>
-      <c r="N26" t="s">
-        <v>1609</v>
-      </c>
-      <c r="O26">
+      <c r="O26" t="s">
+        <v>1588</v>
+      </c>
+      <c r="P26">
         <v>36.095348999999999</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>-82.265000000000001</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>1</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>989</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>22</v>
       </c>
-      <c r="U26" t="s">
-        <v>1610</v>
-      </c>
       <c r="V26" t="s">
-        <v>1611</v>
+        <v>1589</v>
       </c>
       <c r="W26" t="s">
+        <v>1590</v>
+      </c>
+      <c r="X26" t="s">
         <v>1426</v>
       </c>
-      <c r="X26" t="s">
-        <v>1612</v>
-      </c>
-      <c r="AD26" t="s">
+      <c r="Y26" t="s">
+        <v>1591</v>
+      </c>
+      <c r="AE26" t="s">
         <v>1243</v>
       </c>
-      <c r="AG26" t="s">
+      <c r="AH26" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="125" t="s">
         <v>881</v>
       </c>
@@ -32437,49 +32514,49 @@
         <v>785</v>
       </c>
       <c r="I27" t="s">
-        <v>1514</v>
-      </c>
-      <c r="J27" t="s">
+        <v>1627</v>
+      </c>
+      <c r="J27">
+        <v>2007</v>
+      </c>
+      <c r="K27" t="s">
         <v>882</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>883</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>884</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>38.896382000000003</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>-120.041629</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>2</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>22</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>887</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>1401</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>1424</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>1498</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>1457</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AC27" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>1243</v>
       </c>
       <c r="AD27" t="s">
         <v>1243</v>
@@ -32487,11 +32564,14 @@
       <c r="AE27" t="s">
         <v>1243</v>
       </c>
-      <c r="AG27" t="s">
+      <c r="AF27" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH27" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="125" t="s">
         <v>1091</v>
       </c>
@@ -32517,67 +32597,70 @@
         <v>785</v>
       </c>
       <c r="I28" t="s">
-        <v>1526</v>
+        <v>1628</v>
       </c>
       <c r="J28" t="s">
+        <v>1615</v>
+      </c>
+      <c r="K28" t="s">
         <v>24</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>1094</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>1092</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>1093</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>1096</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>40.262369999999997</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>-105.59080400000001</v>
       </c>
-      <c r="Q28" s="100">
+      <c r="R28" s="100">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="U28" t="s">
+      <c r="V28" t="s">
         <v>1095</v>
       </c>
-      <c r="V28" t="s">
+      <c r="W28" t="s">
         <v>1382</v>
       </c>
-      <c r="W28" t="s">
+      <c r="X28" t="s">
         <v>1436</v>
       </c>
-      <c r="X28" t="s">
+      <c r="Y28" t="s">
         <v>1437</v>
       </c>
-      <c r="Y28" s="96" t="s">
+      <c r="Z28" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z28" s="96" t="s">
+      <c r="AA28" s="96" t="s">
         <v>1493</v>
       </c>
-      <c r="AB28" t="s">
+      <c r="AC28" t="s">
         <v>1156</v>
       </c>
-      <c r="AC28" t="s">
+      <c r="AD28" t="s">
         <v>1490</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>1243</v>
       </c>
       <c r="AE28" t="s">
         <v>1243</v>
       </c>
-      <c r="AG28" t="s">
+      <c r="AF28" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH28" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="125" t="s">
         <v>689</v>
       </c>
@@ -32603,70 +32686,73 @@
         <v>693</v>
       </c>
       <c r="I29" t="s">
-        <v>1511</v>
-      </c>
-      <c r="J29" t="s">
+        <v>695</v>
+      </c>
+      <c r="J29">
+        <v>2002</v>
+      </c>
+      <c r="K29" t="s">
         <v>24</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>694</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>19</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>695</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>39.177683000000002</v>
       </c>
-      <c r="P29">
+      <c r="Q29">
         <v>-105.26552</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>5</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>690</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>22</v>
       </c>
-      <c r="U29" t="s">
+      <c r="V29" t="s">
         <v>696</v>
       </c>
-      <c r="V29" t="s">
+      <c r="W29" t="s">
         <v>1382</v>
       </c>
-      <c r="W29" t="s">
+      <c r="X29" t="s">
         <v>1439</v>
       </c>
-      <c r="X29" t="s">
+      <c r="Y29" t="s">
         <v>1438</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Z29" t="s">
         <v>1156</v>
       </c>
-      <c r="Z29" s="115" t="s">
+      <c r="AA29" s="115" t="s">
         <v>1493</v>
       </c>
-      <c r="AB29" t="s">
+      <c r="AC29" t="s">
         <v>1156</v>
       </c>
-      <c r="AC29" t="s">
+      <c r="AD29" t="s">
         <v>1244</v>
       </c>
-      <c r="AD29" t="s">
-        <v>1617</v>
-      </c>
       <c r="AE29" t="s">
+        <v>1596</v>
+      </c>
+      <c r="AF29" t="s">
         <v>1243</v>
       </c>
-      <c r="AG29" t="s">
+      <c r="AH29" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" s="125" t="s">
         <v>762</v>
       </c>
@@ -32692,55 +32778,55 @@
         <v>785</v>
       </c>
       <c r="I30" t="s">
-        <v>1511</v>
-      </c>
-      <c r="J30" t="s">
+        <v>695</v>
+      </c>
+      <c r="J30">
+        <v>2002</v>
+      </c>
+      <c r="K30" t="s">
         <v>24</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>694</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>19</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>721</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>39.177683000000002</v>
       </c>
-      <c r="P30">
+      <c r="Q30">
         <v>-105.26552</v>
-      </c>
-      <c r="S30" t="s">
-        <v>22</v>
       </c>
       <c r="T30" t="s">
         <v>22</v>
       </c>
       <c r="U30" t="s">
+        <v>22</v>
+      </c>
+      <c r="V30" t="s">
         <v>1108</v>
       </c>
-      <c r="V30" t="s">
+      <c r="W30" t="s">
         <v>1382</v>
       </c>
-      <c r="W30" t="s">
+      <c r="X30" t="s">
         <v>1440</v>
       </c>
-      <c r="X30" t="s">
+      <c r="Y30" t="s">
         <v>1441</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>1156</v>
       </c>
-      <c r="Z30" t="s">
+      <c r="AA30" t="s">
         <v>1494</v>
       </c>
-      <c r="AB30" t="s">
+      <c r="AC30" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC30" t="s">
-        <v>1243</v>
       </c>
       <c r="AD30" t="s">
         <v>1243</v>
@@ -32748,11 +32834,14 @@
       <c r="AE30" t="s">
         <v>1243</v>
       </c>
-      <c r="AG30" t="s">
+      <c r="AF30" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH30" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="125" t="s">
         <v>924</v>
       </c>
@@ -32778,67 +32867,67 @@
         <v>785</v>
       </c>
       <c r="I31" t="s">
-        <v>1513</v>
-      </c>
-      <c r="J31" t="s">
+        <v>1511</v>
+      </c>
+      <c r="K31" t="s">
         <v>873</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>926</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>927</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>37.534036999999998</v>
       </c>
-      <c r="P31">
+      <c r="Q31">
         <v>-119.389139</v>
-      </c>
-      <c r="S31" t="s">
-        <v>22</v>
       </c>
       <c r="T31" t="s">
         <v>22</v>
       </c>
       <c r="U31" t="s">
+        <v>22</v>
+      </c>
+      <c r="V31" t="s">
         <v>925</v>
       </c>
-      <c r="V31" t="s">
+      <c r="W31" t="s">
         <v>1401</v>
       </c>
-      <c r="W31" t="s">
+      <c r="X31" t="s">
         <v>1426</v>
       </c>
-      <c r="X31" t="s">
+      <c r="Y31" t="s">
         <v>1427</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>1156</v>
       </c>
-      <c r="Z31" s="116" t="s">
+      <c r="AA31" s="116" t="s">
         <v>1495</v>
       </c>
-      <c r="AB31" t="s">
+      <c r="AC31" t="s">
         <v>1156</v>
       </c>
-      <c r="AC31" t="s">
+      <c r="AD31" t="s">
         <v>1483</v>
       </c>
-      <c r="AD31" t="s">
-        <v>1618</v>
-      </c>
       <c r="AE31" t="s">
+        <v>1597</v>
+      </c>
+      <c r="AF31" t="s">
         <v>1243</v>
       </c>
-      <c r="AF31" t="s">
-        <v>1622</v>
-      </c>
       <c r="AG31" t="s">
+        <v>1601</v>
+      </c>
+      <c r="AH31" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" s="125" t="s">
         <v>948</v>
       </c>
@@ -32861,129 +32950,135 @@
         <v>785</v>
       </c>
       <c r="I32" t="s">
-        <v>1527</v>
-      </c>
-      <c r="M32" t="s">
+        <v>1629</v>
+      </c>
+      <c r="J32">
+        <v>2002</v>
+      </c>
+      <c r="N32" t="s">
         <v>930</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>949</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>44.578524999999999</v>
       </c>
-      <c r="P32">
+      <c r="Q32">
         <v>-115.66604</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <v>4</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>22</v>
       </c>
-      <c r="U32" t="s">
+      <c r="V32" t="s">
         <v>950</v>
       </c>
-      <c r="V32" t="s">
+      <c r="W32" t="s">
         <v>1386</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>1426</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>1427</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>1156</v>
       </c>
-      <c r="Z32" s="116" t="s">
+      <c r="AA32" s="116" t="s">
         <v>1496</v>
       </c>
-      <c r="AB32" t="s">
+      <c r="AC32" t="s">
         <v>1156</v>
       </c>
-      <c r="AC32" t="s">
+      <c r="AD32" t="s">
         <v>1244</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>1243</v>
       </c>
       <c r="AE32" t="s">
         <v>1243</v>
       </c>
-      <c r="AF32" s="8" t="s">
+      <c r="AF32" t="s">
+        <v>1243</v>
+      </c>
+      <c r="AG32" s="8" t="s">
         <v>1488</v>
       </c>
-      <c r="AG32" s="8" t="s">
+      <c r="AH32" s="8" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33" s="125" t="s">
-        <v>1585</v>
+        <v>1566</v>
       </c>
       <c r="B33">
         <v>1973</v>
       </c>
       <c r="C33" t="s">
-        <v>1586</v>
+        <v>1567</v>
       </c>
       <c r="I33" t="s">
-        <v>1587</v>
-      </c>
-      <c r="J33" t="s">
+        <v>1630</v>
+      </c>
+      <c r="J33">
+        <v>1970</v>
+      </c>
+      <c r="K33" t="s">
         <v>24</v>
       </c>
-      <c r="K33" t="s">
-        <v>1588</v>
-      </c>
       <c r="L33" t="s">
+        <v>1568</v>
+      </c>
+      <c r="M33" t="s">
         <v>19</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>883</v>
       </c>
-      <c r="N33" t="s">
-        <v>1589</v>
-      </c>
-      <c r="O33" s="122">
+      <c r="O33" t="s">
+        <v>1569</v>
+      </c>
+      <c r="P33" s="122">
         <v>48.102674999999998</v>
       </c>
-      <c r="P33" s="122">
+      <c r="Q33" s="122">
         <v>-120.35232000000001</v>
       </c>
-      <c r="Q33">
+      <c r="R33">
         <v>2</v>
       </c>
-      <c r="R33" t="s">
-        <v>1590</v>
-      </c>
-      <c r="T33" t="s">
+      <c r="S33" t="s">
+        <v>1570</v>
+      </c>
+      <c r="U33" t="s">
         <v>22</v>
       </c>
-      <c r="U33" t="s">
-        <v>1591</v>
-      </c>
       <c r="V33" t="s">
+        <v>1571</v>
+      </c>
+      <c r="W33" t="s">
         <v>1401</v>
       </c>
-      <c r="W33" t="s">
+      <c r="X33" t="s">
         <v>1426</v>
       </c>
-      <c r="X33" t="s">
-        <v>1592</v>
-      </c>
-      <c r="AD33" t="s">
-        <v>1243</v>
+      <c r="Y33" t="s">
+        <v>1572</v>
       </c>
       <c r="AE33" t="s">
         <v>1243</v>
       </c>
-      <c r="AG33" t="s">
+      <c r="AF33" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH33" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34" s="125" t="s">
         <v>871</v>
       </c>
@@ -33009,68 +33104,71 @@
         <v>785</v>
       </c>
       <c r="I34" s="96" t="s">
-        <v>1525</v>
-      </c>
-      <c r="J34" t="s">
+        <v>1631</v>
+      </c>
+      <c r="J34" s="96">
+        <v>2015</v>
+      </c>
+      <c r="K34" t="s">
         <v>873</v>
       </c>
-      <c r="M34" s="104" t="s">
+      <c r="N34" s="104" t="s">
         <v>874</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>875</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>38.512031</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <v>-122.097228</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <v>3</v>
       </c>
-      <c r="R34" t="s">
+      <c r="S34" t="s">
         <v>876</v>
-      </c>
-      <c r="S34" t="s">
-        <v>22</v>
       </c>
       <c r="T34" t="s">
         <v>22</v>
       </c>
       <c r="U34" t="s">
+        <v>22</v>
+      </c>
+      <c r="V34" t="s">
         <v>872</v>
       </c>
-      <c r="V34" t="s">
+      <c r="W34" t="s">
         <v>1401</v>
       </c>
-      <c r="W34" t="s">
+      <c r="X34" t="s">
         <v>1422</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Y34" t="s">
         <v>1428</v>
       </c>
-      <c r="Y34" s="96" t="s">
+      <c r="Z34" s="96" t="s">
         <v>1477</v>
       </c>
-      <c r="Z34" s="96"/>
-      <c r="AB34" t="s">
+      <c r="AA34" s="96"/>
+      <c r="AC34" t="s">
         <v>1156</v>
       </c>
-      <c r="AC34" t="s">
+      <c r="AD34" t="s">
         <v>1487</v>
       </c>
-      <c r="AD34" t="s">
+      <c r="AE34" t="s">
         <v>1485</v>
       </c>
-      <c r="AE34" t="s">
+      <c r="AF34" t="s">
         <v>1243</v>
       </c>
-      <c r="AG34" t="s">
+      <c r="AH34" t="s">
         <v>1243</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35" s="125" t="s">
         <v>765</v>
       </c>
@@ -33096,61 +33194,61 @@
         <v>785</v>
       </c>
       <c r="I35" t="s">
-        <v>1512</v>
-      </c>
-      <c r="J35" s="108" t="s">
+        <v>1632</v>
+      </c>
+      <c r="J35" s="96">
+        <v>2012</v>
+      </c>
+      <c r="K35" s="108" t="s">
         <v>770</v>
       </c>
-      <c r="K35" s="108" t="s">
+      <c r="L35" s="108" t="s">
         <v>771</v>
       </c>
-      <c r="L35" s="108" t="s">
+      <c r="M35" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <v>1</v>
       </c>
-      <c r="N35" s="108" t="s">
+      <c r="O35" s="108" t="s">
         <v>767</v>
       </c>
-      <c r="O35" s="109">
+      <c r="P35" s="109">
         <v>40.7159999</v>
       </c>
-      <c r="P35" s="109">
+      <c r="Q35" s="109">
         <v>-105.23308400000001</v>
       </c>
-      <c r="Q35" s="110">
+      <c r="R35" s="110">
         <v>0.5</v>
       </c>
-      <c r="R35" s="110" t="s">
+      <c r="S35" s="110" t="s">
         <v>768</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>22</v>
       </c>
-      <c r="U35" t="s">
+      <c r="V35" t="s">
         <v>769</v>
       </c>
-      <c r="V35" t="s">
+      <c r="W35" t="s">
         <v>1382</v>
       </c>
-      <c r="W35" t="s">
+      <c r="X35" t="s">
         <v>1430</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Y35" t="s">
         <v>1442</v>
       </c>
-      <c r="Y35" s="96" t="s">
+      <c r="Z35" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z35" s="96" t="s">
+      <c r="AA35" s="96" t="s">
         <v>1492</v>
       </c>
-      <c r="AB35" t="s">
+      <c r="AC35" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC35" t="s">
-        <v>1243</v>
       </c>
       <c r="AD35" t="s">
         <v>1243</v>
@@ -33158,11 +33256,14 @@
       <c r="AE35" t="s">
         <v>1243</v>
       </c>
-      <c r="AG35" t="s">
+      <c r="AF35" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH35" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36" s="125" t="s">
         <v>1232</v>
       </c>
@@ -33173,38 +33274,41 @@
         <v>1451</v>
       </c>
       <c r="I36" s="96" t="s">
-        <v>1524</v>
-      </c>
-      <c r="W36" t="s">
+        <v>1626</v>
+      </c>
+      <c r="J36" s="96">
+        <v>2010</v>
+      </c>
+      <c r="X36" t="s">
         <v>1422</v>
       </c>
-      <c r="X36" t="s">
+      <c r="Y36" t="s">
         <v>1452</v>
       </c>
-      <c r="Y36" s="96" t="s">
+      <c r="Z36" s="96" t="s">
         <v>1478</v>
       </c>
-      <c r="Z36" s="96"/>
-      <c r="AB36" t="s">
+      <c r="AA36" s="96"/>
+      <c r="AC36" t="s">
         <v>1156</v>
       </c>
-      <c r="AC36" t="s">
+      <c r="AD36" t="s">
         <v>1488</v>
       </c>
-      <c r="AD36" t="s">
-        <v>1619</v>
-      </c>
       <c r="AE36" t="s">
+        <v>1598</v>
+      </c>
+      <c r="AF36" t="s">
         <v>1243</v>
       </c>
-      <c r="AF36" s="8" t="s">
+      <c r="AG36" s="8" t="s">
         <v>1488</v>
       </c>
-      <c r="AG36" s="8" t="s">
+      <c r="AH36" s="8" t="s">
         <v>1244</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37" s="125" t="s">
         <v>789</v>
       </c>
@@ -33229,60 +33333,60 @@
       <c r="I37" t="s">
         <v>1510</v>
       </c>
-      <c r="J37" s="96" t="s">
+      <c r="J37" t="s">
+        <v>1633</v>
+      </c>
+      <c r="K37" s="96" t="s">
         <v>770</v>
       </c>
-      <c r="K37" s="96" t="s">
+      <c r="L37" s="96" t="s">
         <v>771</v>
       </c>
-      <c r="L37" s="96" t="s">
+      <c r="M37" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="M37" s="96"/>
-      <c r="N37" s="96" t="s">
+      <c r="N37" s="96"/>
+      <c r="O37" s="96" t="s">
         <v>767</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>40.702464999999997</v>
       </c>
-      <c r="P37">
+      <c r="Q37">
         <v>-105.241646</v>
       </c>
-      <c r="Q37">
+      <c r="R37">
         <v>1</v>
       </c>
-      <c r="R37" t="s">
+      <c r="S37" t="s">
         <v>790</v>
-      </c>
-      <c r="S37" t="s">
-        <v>22</v>
       </c>
       <c r="T37" t="s">
         <v>22</v>
       </c>
       <c r="U37" t="s">
+        <v>22</v>
+      </c>
+      <c r="V37" t="s">
         <v>791</v>
       </c>
-      <c r="V37" t="s">
+      <c r="W37" t="s">
         <v>1401</v>
       </c>
-      <c r="W37" t="s">
+      <c r="X37" t="s">
         <v>1430</v>
       </c>
-      <c r="X37" t="s">
+      <c r="Y37" t="s">
         <v>1429</v>
       </c>
-      <c r="Y37" s="96" t="s">
+      <c r="Z37" s="96" t="s">
         <v>1156</v>
       </c>
-      <c r="Z37" s="96" t="s">
+      <c r="AA37" s="96" t="s">
         <v>1492</v>
       </c>
-      <c r="AB37" t="s">
+      <c r="AC37" t="s">
         <v>1156</v>
-      </c>
-      <c r="AC37" t="s">
-        <v>1243</v>
       </c>
       <c r="AD37" t="s">
         <v>1243</v>
@@ -33290,12 +33394,15 @@
       <c r="AE37" t="s">
         <v>1243</v>
       </c>
-      <c r="AG37" t="s">
+      <c r="AF37" t="s">
         <v>1243</v>
       </c>
+      <c r="AH37" t="s">
+        <v>1243</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE37">
     <sortCondition ref="B2:B37"/>
   </sortState>
   <dataValidations count="3">
@@ -33335,16 +33442,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>1532</v>
+        <v>1513</v>
       </c>
       <c r="B1" s="105" t="s">
-        <v>1533</v>
+        <v>1514</v>
       </c>
       <c r="C1" t="s">
-        <v>1572</v>
+        <v>1553</v>
       </c>
       <c r="D1" s="105" t="s">
-        <v>1569</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -33352,10 +33459,10 @@
         <v>935</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>1559</v>
+        <v>1540</v>
       </c>
       <c r="D2" s="117" t="s">
-        <v>1559</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -33363,7 +33470,7 @@
         <v>1174</v>
       </c>
       <c r="B3" s="118" t="s">
-        <v>1546</v>
+        <v>1527</v>
       </c>
       <c r="D3" s="60" t="s">
         <v>681</v>
@@ -33374,10 +33481,10 @@
         <v>681</v>
       </c>
       <c r="B4" s="119" t="s">
-        <v>1560</v>
+        <v>1541</v>
       </c>
       <c r="C4" t="s">
-        <v>1573</v>
+        <v>1554</v>
       </c>
       <c r="D4" t="s">
         <v>1413</v>
@@ -33388,10 +33495,10 @@
         <v>681</v>
       </c>
       <c r="B5" s="119" t="s">
-        <v>1564</v>
+        <v>1545</v>
       </c>
       <c r="C5" t="s">
-        <v>1574</v>
+        <v>1555</v>
       </c>
       <c r="D5" t="s">
         <v>1443</v>
@@ -33402,7 +33509,7 @@
         <v>1404</v>
       </c>
       <c r="B6" s="118" t="s">
-        <v>1541</v>
+        <v>1522</v>
       </c>
       <c r="D6" t="s">
         <v>928</v>
@@ -33413,10 +33520,10 @@
         <v>1413</v>
       </c>
       <c r="B7" s="120" t="s">
-        <v>1542</v>
+        <v>1523</v>
       </c>
       <c r="C7" t="s">
-        <v>1575</v>
+        <v>1556</v>
       </c>
       <c r="D7" t="s">
         <v>727</v>
@@ -33427,10 +33534,10 @@
         <v>835</v>
       </c>
       <c r="B8" s="119" t="s">
-        <v>1549</v>
+        <v>1530</v>
       </c>
       <c r="C8" t="s">
-        <v>1576</v>
+        <v>1557</v>
       </c>
       <c r="D8" t="s">
         <v>1231</v>
@@ -33441,10 +33548,10 @@
         <v>1001</v>
       </c>
       <c r="B9" s="119" t="s">
-        <v>1549</v>
+        <v>1530</v>
       </c>
       <c r="C9" t="s">
-        <v>1577</v>
+        <v>1558</v>
       </c>
       <c r="D9" t="s">
         <v>1233</v>
@@ -33455,10 +33562,10 @@
         <v>982</v>
       </c>
       <c r="B10" s="119" t="s">
-        <v>1561</v>
+        <v>1542</v>
       </c>
       <c r="C10" t="s">
-        <v>1578</v>
+        <v>1559</v>
       </c>
       <c r="D10" s="96" t="s">
         <v>750</v>
@@ -33469,10 +33576,10 @@
         <v>1443</v>
       </c>
       <c r="B11" s="119" t="s">
-        <v>1552</v>
+        <v>1533</v>
       </c>
       <c r="C11" t="s">
-        <v>1579</v>
+        <v>1560</v>
       </c>
       <c r="D11" s="96" t="s">
         <v>826</v>
@@ -33483,10 +33590,10 @@
         <v>928</v>
       </c>
       <c r="B12" s="119" t="s">
-        <v>1544</v>
+        <v>1525</v>
       </c>
       <c r="C12" t="s">
-        <v>1580</v>
+        <v>1561</v>
       </c>
       <c r="D12" t="s">
         <v>711</v>
@@ -33497,7 +33604,7 @@
         <v>670</v>
       </c>
       <c r="B13" s="118" t="s">
-        <v>1556</v>
+        <v>1537</v>
       </c>
       <c r="D13" t="s">
         <v>881</v>
@@ -33508,10 +33615,10 @@
         <v>909</v>
       </c>
       <c r="B14" s="123" t="s">
-        <v>1562</v>
+        <v>1543</v>
       </c>
       <c r="C14" t="s">
-        <v>1603</v>
+        <v>1582</v>
       </c>
       <c r="D14" t="s">
         <v>762</v>
@@ -33522,7 +33629,7 @@
         <v>1183</v>
       </c>
       <c r="B15" s="118" t="s">
-        <v>1557</v>
+        <v>1538</v>
       </c>
       <c r="D15" t="s">
         <v>789</v>
@@ -33533,7 +33640,7 @@
         <v>727</v>
       </c>
       <c r="B16" s="118" t="s">
-        <v>1535</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -33541,10 +33648,10 @@
         <v>1165</v>
       </c>
       <c r="B17" s="118" t="s">
-        <v>1537</v>
+        <v>1518</v>
       </c>
       <c r="D17" t="s">
-        <v>1570</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -33552,13 +33659,13 @@
         <v>1231</v>
       </c>
       <c r="B18" s="119" t="s">
-        <v>1568</v>
+        <v>1549</v>
       </c>
       <c r="C18" t="s">
         <v>700</v>
       </c>
       <c r="D18" t="s">
-        <v>1571</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -33566,10 +33673,10 @@
         <v>720</v>
       </c>
       <c r="B19" s="119" t="s">
-        <v>1545</v>
+        <v>1526</v>
       </c>
       <c r="C19" t="s">
-        <v>1576</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -33577,10 +33684,10 @@
         <v>1233</v>
       </c>
       <c r="B20" s="119" t="s">
-        <v>1563</v>
+        <v>1544</v>
       </c>
       <c r="C20" t="s">
-        <v>1581</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -33588,7 +33695,7 @@
         <v>750</v>
       </c>
       <c r="B21" s="118" t="s">
-        <v>1547</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -33596,7 +33703,7 @@
         <v>826</v>
       </c>
       <c r="B22" s="118" t="s">
-        <v>1536</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -33604,7 +33711,7 @@
         <v>711</v>
       </c>
       <c r="B23" s="118" t="s">
-        <v>1538</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -33612,10 +33719,10 @@
         <v>848</v>
       </c>
       <c r="B24" s="121" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C24" t="s">
         <v>1565</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1584</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -33623,7 +33730,7 @@
         <v>881</v>
       </c>
       <c r="B25" s="118" t="s">
-        <v>1543</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -33631,10 +33738,10 @@
         <v>1091</v>
       </c>
       <c r="B26" s="119" t="s">
-        <v>1553</v>
+        <v>1534</v>
       </c>
       <c r="C26" t="s">
-        <v>1576</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -33642,7 +33749,7 @@
         <v>689</v>
       </c>
       <c r="B27" s="118" t="s">
-        <v>1534</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -33650,10 +33757,10 @@
         <v>762</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>1540</v>
+        <v>1521</v>
       </c>
       <c r="C28" t="s">
-        <v>1582</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -33661,10 +33768,10 @@
         <v>924</v>
       </c>
       <c r="B29" s="119" t="s">
-        <v>1550</v>
+        <v>1531</v>
       </c>
       <c r="C29" t="s">
-        <v>1578</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -33672,10 +33779,10 @@
         <v>948</v>
       </c>
       <c r="B30" s="119" t="s">
-        <v>1554</v>
+        <v>1535</v>
       </c>
       <c r="C30" t="s">
-        <v>1583</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -33683,10 +33790,10 @@
         <v>871</v>
       </c>
       <c r="B31" s="123" t="s">
-        <v>1567</v>
+        <v>1548</v>
       </c>
       <c r="C31" t="s">
-        <v>1593</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -33694,10 +33801,10 @@
         <v>765</v>
       </c>
       <c r="B32" s="119" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C32" t="s">
         <v>1555</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1574</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -33705,10 +33812,10 @@
         <v>1232</v>
       </c>
       <c r="B33" s="119" t="s">
-        <v>1551</v>
+        <v>1532</v>
       </c>
       <c r="C33" t="s">
-        <v>1574</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -33716,31 +33823,31 @@
         <v>789</v>
       </c>
       <c r="B34" s="119" t="s">
-        <v>1548</v>
+        <v>1529</v>
       </c>
       <c r="C34" t="s">
-        <v>1574</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B35" s="119" t="s">
-        <v>1558</v>
+        <v>1539</v>
       </c>
       <c r="C35" t="s">
-        <v>1578</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B36" s="119" t="s">
-        <v>1566</v>
+        <v>1547</v>
       </c>
       <c r="C36" t="s">
-        <v>1576</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B37" s="118" t="s">
-        <v>1539</v>
+        <v>1520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checking on Confidence Intervals
</commit_message>
<xml_diff>
--- a/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
+++ b/FireMeta_Rproj/inputs/StudiesData_Table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cava304/GitHub/rc_sfa-rc-3-wenas-meta/FireMeta_Rproj/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF87A9E-D152-194D-91AC-BDB6C99AFE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26549174-45E8-4446-8173-55E1814FFB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="7" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="7" xr2:uid="{4E0DEC49-1D65-E841-934F-3D87EA14399D}"/>
   </bookViews>
   <sheets>
     <sheet name="Study_info" sheetId="2" r:id="rId1"/>
@@ -5514,7 +5514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -5684,16 +5684,10 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -30551,9 +30545,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E83DAFB-3D69-1A4C-8997-3EF8B4236F27}">
   <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I40" sqref="I40"/>
+      <selection pane="topRight" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34470,8 +34464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F57175-4851-C144-BE97-0FB64AE1A031}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34498,7 +34492,7 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="133" t="s">
+      <c r="D1" s="129" t="s">
         <v>16</v>
       </c>
     </row>
@@ -34548,7 +34542,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="129" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="127" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="126" t="s">
         <v>1413</v>
       </c>
@@ -34558,15 +34552,15 @@
       <c r="C7" s="128" t="s">
         <v>1636</v>
       </c>
-      <c r="D7" s="129" t="s">
+      <c r="D7" s="127" t="s">
         <v>1660</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="125" t="s">
         <v>835</v>
       </c>
-      <c r="B8" s="132" t="s">
+      <c r="B8" t="s">
         <v>1639</v>
       </c>
       <c r="D8" t="s">
@@ -34579,31 +34573,31 @@
         <v>766</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="126" t="s">
         <v>1001</v>
       </c>
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="128" t="s">
         <v>1648</v>
       </c>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="127" t="s">
         <v>1656</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="126" t="s">
         <v>982</v>
       </c>
-      <c r="B10" s="129" t="s">
+      <c r="B10" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C10" s="130" t="s">
+      <c r="C10" s="128" t="s">
         <v>1636</v>
       </c>
-      <c r="D10" s="129" t="s">
+      <c r="D10" s="127" t="s">
         <v>1657</v>
       </c>
     </row>
@@ -34675,45 +34669,45 @@
         <v>766</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="126" t="s">
         <v>670</v>
       </c>
-      <c r="B15" s="129" t="s">
+      <c r="B15" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="128" t="s">
         <v>1636</v>
       </c>
-      <c r="D15" s="129" t="s">
+      <c r="D15" s="127" t="s">
         <v>1649</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="126" t="s">
         <v>909</v>
       </c>
-      <c r="B16" s="129" t="s">
+      <c r="B16" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C16" s="130" t="s">
+      <c r="C16" s="128" t="s">
         <v>1636</v>
       </c>
-      <c r="D16" s="129" t="s">
+      <c r="D16" s="127" t="s">
         <v>1658</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="126" t="s">
         <v>1183</v>
       </c>
-      <c r="B17" s="129" t="s">
+      <c r="B17" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C17" s="130" t="s">
+      <c r="C17" s="128" t="s">
         <v>1636</v>
       </c>
-      <c r="D17" s="129" t="s">
+      <c r="D17" s="127" t="s">
         <v>1659</v>
       </c>
     </row>
@@ -34759,17 +34753,17 @@
         <v>692</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="126" t="s">
         <v>1233</v>
       </c>
-      <c r="B21" s="129" t="s">
+      <c r="B21" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C21" s="130" t="s">
+      <c r="C21" s="128" t="s">
         <v>1636</v>
       </c>
-      <c r="D21" s="129" t="s">
+      <c r="D21" s="127" t="s">
         <v>1659</v>
       </c>
     </row>
@@ -34891,45 +34885,45 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="126" t="s">
         <v>762</v>
       </c>
-      <c r="B30" s="129" t="s">
+      <c r="B30" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C30" s="130" t="s">
+      <c r="C30" s="128" t="s">
         <v>1636</v>
       </c>
-      <c r="D30" s="129" t="s">
+      <c r="D30" s="127" t="s">
         <v>1658</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="126" t="s">
         <v>924</v>
       </c>
-      <c r="B31" s="129" t="s">
+      <c r="B31" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C31" s="130" t="s">
+      <c r="C31" s="128" t="s">
         <v>1636</v>
       </c>
-      <c r="D31" s="129" t="s">
+      <c r="D31" s="127" t="s">
         <v>1658</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="126" t="s">
         <v>948</v>
       </c>
-      <c r="B32" s="129" t="s">
+      <c r="B32" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C32" s="130" t="s">
+      <c r="C32" s="128" t="s">
         <v>1648</v>
       </c>
-      <c r="D32" s="129" t="s">
+      <c r="D32" s="127" t="s">
         <v>1661</v>
       </c>
     </row>
@@ -34984,17 +34978,17 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="129" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="126" t="s">
         <v>1232</v>
       </c>
-      <c r="B36" s="129" t="s">
+      <c r="B36" s="127" t="s">
         <v>1637</v>
       </c>
-      <c r="C36" s="130" t="s">
+      <c r="C36" s="128" t="s">
         <v>1648</v>
       </c>
-      <c r="D36" s="129" t="s">
+      <c r="D36" s="127" t="s">
         <v>1656</v>
       </c>
     </row>

</xml_diff>